<commit_message>
converted docker container to singularity for MPI hello world
</commit_message>
<xml_diff>
--- a/Containers/First experiments/results/results.xlsx
+++ b/Containers/First experiments/results/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karahbit/koubbe/Containers/First experiments/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F338DD-DC48-C443-8853-30C2930A5990}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2C8B18-9261-9945-9376-DB93B9AD2DCF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="460" windowWidth="37540" windowHeight="21140" xr2:uid="{5C86F751-EA59-464C-941B-333EDFC81949}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{5C86F751-EA59-464C-941B-333EDFC81949}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="24">
   <si>
     <t>non-containerized</t>
   </si>
@@ -63,10 +63,40 @@
     <t>Std Dev</t>
   </si>
   <si>
-    <t>16</t>
+    <t>1/1/1</t>
   </si>
   <si>
-    <t>32</t>
+    <t>2/2/1</t>
+  </si>
+  <si>
+    <t>4/4/1</t>
+  </si>
+  <si>
+    <t>8/8/1</t>
+  </si>
+  <si>
+    <t>16/16/1</t>
+  </si>
+  <si>
+    <t>32/32/2</t>
+  </si>
+  <si>
+    <t>56/1/2</t>
+  </si>
+  <si>
+    <t>112/2/4</t>
+  </si>
+  <si>
+    <t>224/4/8</t>
+  </si>
+  <si>
+    <t>448/8/16</t>
+  </si>
+  <si>
+    <t>896/16/32</t>
+  </si>
+  <si>
+    <t>1792/32/64</t>
   </si>
 </sst>
 </file>
@@ -122,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -130,14 +160,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -258,22 +291,8 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -390,6 +409,10 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -652,6 +675,24 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
@@ -804,6 +845,27 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
@@ -880,6 +942,82 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1131,6 +1269,7 @@
       </font>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1302,8 +1441,85 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1477,359 +1693,182 @@
       </font>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2064,16 +2103,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1/1/1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2/2/1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4/4/1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8/8/1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2286,16 +2325,16 @@
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1/1/1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2/2/1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4/4/1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8/8/1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2368,7 +2407,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Number of cores</a:t>
+                  <a:t>cores/tasks/nodes</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2420,7 +2459,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -2870,22 +2909,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1/1/1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2/2/1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4/4/1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8/8/1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16/16/1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32/32/2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3074,22 +3113,22 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>1/1/1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2/2/1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>4/4/1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>8/8/1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>16/16/1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>32/32/2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3168,7 +3207,693 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Number of cores</a:t>
+                  <a:t>cores/tasks/nodes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1766352896"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1766352896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>TTX</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (seconds)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1743758432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>MPI Hello World on Bridges using Singularity</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>non-containerized</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$C$99:$H$99</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$C$99:$H$99</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$87:$H$87</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>56/1/2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>112/2/4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>224/4/8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>448/8/16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>896/16/32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1792/32/64</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$98:$H$98</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-10FA-5D49-8521-CD792A8DB53D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>containerized</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$L$99:$Q$99</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$L$99:$Q$99</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$87:$H$87</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>56/1/2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>112/2/4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>224/4/8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>448/8/16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>896/16/32</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1792/32/64</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$98:$Q$98</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-10FA-5D49-8521-CD792A8DB53D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1743758432"/>
+        <c:axId val="1766352896"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1743758432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>cores/tasks/nodes</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -3518,6 +4243,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -4022,6 +4787,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4600,11 +5868,49 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C93F5EC-6D90-8C4E-AC07-BA547878C61D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{AB51CF61-79E3-FF4F-B384-F02243D3273A}" name="Table12" displayName="Table12" ref="L8:O19" totalsRowCount="1" headerRowDxfId="94" dataDxfId="95">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{AB51CF61-79E3-FF4F-B384-F02243D3273A}" name="Table12" displayName="Table12" ref="L8:O19" totalsRowCount="1" headerRowDxfId="95" dataDxfId="94">
   <autoFilter ref="L8:O18" xr:uid="{4157A701-19DE-9F43-9C32-34B7BD7CBED0}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4612,19 +5918,19 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A2B04CA0-9DF0-5F41-B767-0E628D6F8EE7}" name="1" totalsRowFunction="custom" dataDxfId="93" totalsRowDxfId="92">
-      <totalsRowFormula>AVERAGE(Table12[1])</totalsRowFormula>
+    <tableColumn id="1" xr3:uid="{A2B04CA0-9DF0-5F41-B767-0E628D6F8EE7}" name="1/1/1" totalsRowFunction="custom" dataDxfId="93" totalsRowDxfId="92">
+      <totalsRowFormula>AVERAGE(Table12[1/1/1])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{C90CC318-E4DA-9B40-A32D-3102841F0921}" name="2" totalsRowFunction="average" dataDxfId="91" totalsRowDxfId="90"/>
-    <tableColumn id="3" xr3:uid="{61A7C00A-F63D-C44A-AFA0-6B9EC0793A33}" name="4" totalsRowFunction="average" dataDxfId="89" totalsRowDxfId="88"/>
-    <tableColumn id="4" xr3:uid="{56012B1C-DD0E-0744-9080-C13899D5A44A}" name="8" totalsRowFunction="average" dataDxfId="87" totalsRowDxfId="86"/>
+    <tableColumn id="2" xr3:uid="{C90CC318-E4DA-9B40-A32D-3102841F0921}" name="2/2/1" totalsRowFunction="average" dataDxfId="91" totalsRowDxfId="90"/>
+    <tableColumn id="3" xr3:uid="{61A7C00A-F63D-C44A-AFA0-6B9EC0793A33}" name="4/4/1" totalsRowFunction="average" dataDxfId="89" totalsRowDxfId="88"/>
+    <tableColumn id="4" xr3:uid="{56012B1C-DD0E-0744-9080-C13899D5A44A}" name="8/8/1" totalsRowFunction="average" dataDxfId="87" totalsRowDxfId="86"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{43882465-33C1-8E45-8C5B-6E2796C69C30}" name="Table1214" displayName="Table1214" ref="C8:F19" totalsRowCount="1" headerRowDxfId="85" dataDxfId="80">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{43882465-33C1-8E45-8C5B-6E2796C69C30}" name="Table1214" displayName="Table1214" ref="C8:F19" totalsRowCount="1" headerRowDxfId="85" dataDxfId="84">
   <autoFilter ref="C8:F18" xr:uid="{26D4EAA6-0F6B-D847-AC4C-A1E1EF972243}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4632,19 +5938,19 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{ECEFB9F6-16FE-E04E-844A-AACC7B293BB2}" name="1" totalsRowFunction="custom" dataDxfId="84" totalsRowDxfId="79">
-      <totalsRowFormula>AVERAGE(Table1214[1])</totalsRowFormula>
+    <tableColumn id="1" xr3:uid="{ECEFB9F6-16FE-E04E-844A-AACC7B293BB2}" name="1/1/1" totalsRowFunction="custom" dataDxfId="83" totalsRowDxfId="82">
+      <totalsRowFormula>AVERAGE(Table1214[1/1/1])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{55F72C56-FCA4-AC43-B626-4AF6B7483939}" name="2" totalsRowFunction="average" dataDxfId="83" totalsRowDxfId="78"/>
-    <tableColumn id="3" xr3:uid="{7C069732-E830-8045-A0B0-B3BF291610EF}" name="4" totalsRowFunction="average" dataDxfId="82" totalsRowDxfId="77"/>
-    <tableColumn id="4" xr3:uid="{8CDDC8E9-E772-C14C-B2C1-6A75594F5FBE}" name="8" totalsRowFunction="average" dataDxfId="81" totalsRowDxfId="76"/>
+    <tableColumn id="2" xr3:uid="{55F72C56-FCA4-AC43-B626-4AF6B7483939}" name="2/2/1" totalsRowFunction="average" dataDxfId="81" totalsRowDxfId="80"/>
+    <tableColumn id="3" xr3:uid="{7C069732-E830-8045-A0B0-B3BF291610EF}" name="4/4/1" totalsRowFunction="average" dataDxfId="79" totalsRowDxfId="78"/>
+    <tableColumn id="4" xr3:uid="{8CDDC8E9-E772-C14C-B2C1-6A75594F5FBE}" name="8/8/1" totalsRowFunction="average" dataDxfId="77" totalsRowDxfId="76"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{FE766060-A7BD-2048-ABFD-3FD69B515A68}" name="Table121415" displayName="Table121415" ref="C35:H46" totalsRowCount="1" headerRowDxfId="75" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{FE766060-A7BD-2048-ABFD-3FD69B515A68}" name="Table121415" displayName="Table121415" ref="C35:H46" totalsRowCount="1" headerRowDxfId="75" dataDxfId="74">
   <autoFilter ref="C35:H45" xr:uid="{B8E8E606-9A74-0D4F-AA01-6A7104D5FDDD}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4654,21 +5960,21 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{5B90E881-6C60-454E-86BB-086695E6CAF8}" name="1" totalsRowFunction="custom" dataDxfId="12" totalsRowDxfId="5">
-      <totalsRowFormula>AVERAGE(Table121415[1])</totalsRowFormula>
+    <tableColumn id="1" xr3:uid="{5B90E881-6C60-454E-86BB-086695E6CAF8}" name="1/1/1" totalsRowFunction="custom" dataDxfId="73" totalsRowDxfId="72">
+      <totalsRowFormula>AVERAGE(Table121415[1/1/1])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{D531CACF-18B4-1041-B0C1-6D0252E32A8A}" name="2" totalsRowFunction="average" dataDxfId="11" totalsRowDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{D0898416-43B5-3E4A-BDC1-7C89C1F0D5E0}" name="4" totalsRowFunction="average" dataDxfId="10" totalsRowDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{4392AEA4-B357-F647-A208-E130D063C6E1}" name="8" totalsRowFunction="average" dataDxfId="9" totalsRowDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{0A1338EF-4B77-1D48-8777-D4CA34460AB0}" name="16" totalsRowFunction="average" dataDxfId="8" totalsRowDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{B90FEE84-6896-1641-8E20-B1872987B7BE}" name="32" totalsRowFunction="average" dataDxfId="7" totalsRowDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{D531CACF-18B4-1041-B0C1-6D0252E32A8A}" name="2/2/1" totalsRowFunction="average" dataDxfId="71" totalsRowDxfId="70"/>
+    <tableColumn id="3" xr3:uid="{D0898416-43B5-3E4A-BDC1-7C89C1F0D5E0}" name="4/4/1" totalsRowFunction="average" dataDxfId="69" totalsRowDxfId="68"/>
+    <tableColumn id="4" xr3:uid="{4392AEA4-B357-F647-A208-E130D063C6E1}" name="8/8/1" totalsRowFunction="average" dataDxfId="67" totalsRowDxfId="66"/>
+    <tableColumn id="6" xr3:uid="{0A1338EF-4B77-1D48-8777-D4CA34460AB0}" name="16/16/1" totalsRowFunction="average" dataDxfId="65" totalsRowDxfId="64"/>
+    <tableColumn id="7" xr3:uid="{B90FEE84-6896-1641-8E20-B1872987B7BE}" name="32/32/2" totalsRowFunction="average" dataDxfId="63" totalsRowDxfId="62"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{C0771168-9D09-C749-AC55-A312881E4A86}" name="Table12141516" displayName="Table12141516" ref="L35:Q46" totalsRowCount="1" headerRowDxfId="74" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{C0771168-9D09-C749-AC55-A312881E4A86}" name="Table12141516" displayName="Table12141516" ref="L35:Q46" totalsRowCount="1" headerRowDxfId="61" dataDxfId="60">
   <autoFilter ref="L35:Q45" xr:uid="{4EFDE026-18DB-0845-B41D-7D7B774A1B01}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4678,21 +5984,21 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{3F8BB35C-BA7F-414F-98E1-50F3192CFD83}" name="1" totalsRowFunction="custom" dataDxfId="25" totalsRowDxfId="18">
-      <totalsRowFormula>AVERAGE(Table12141516[1])</totalsRowFormula>
+    <tableColumn id="1" xr3:uid="{3F8BB35C-BA7F-414F-98E1-50F3192CFD83}" name="1/1/1" totalsRowFunction="custom" dataDxfId="59" totalsRowDxfId="58">
+      <totalsRowFormula>AVERAGE(Table12141516[1/1/1])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{070B7708-5F3C-5747-BB02-C79FC61D286A}" name="2" totalsRowFunction="average" dataDxfId="24" totalsRowDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{58E0425E-3A2E-5C45-8330-41CFB638FBEE}" name="4" totalsRowFunction="average" dataDxfId="23" totalsRowDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{21D6854D-0C08-4B4A-86CE-586C1F6F99EF}" name="8" totalsRowFunction="average" dataDxfId="22" totalsRowDxfId="15"/>
-    <tableColumn id="6" xr3:uid="{6E478822-1027-2D40-94B7-591A68C43394}" name="16" totalsRowFunction="average" dataDxfId="21" totalsRowDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{063A683F-E92B-DC4C-8BF0-A3E1B5948664}" name="32" totalsRowFunction="average" dataDxfId="20" totalsRowDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{070B7708-5F3C-5747-BB02-C79FC61D286A}" name="2/2/1" totalsRowFunction="average" dataDxfId="57" totalsRowDxfId="56"/>
+    <tableColumn id="3" xr3:uid="{58E0425E-3A2E-5C45-8330-41CFB638FBEE}" name="4/4/1" totalsRowFunction="average" dataDxfId="55" totalsRowDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{21D6854D-0C08-4B4A-86CE-586C1F6F99EF}" name="8/8/1" totalsRowFunction="average" dataDxfId="53" totalsRowDxfId="52"/>
+    <tableColumn id="6" xr3:uid="{6E478822-1027-2D40-94B7-591A68C43394}" name="16/16/1" totalsRowFunction="average" dataDxfId="51" totalsRowDxfId="50"/>
+    <tableColumn id="7" xr3:uid="{063A683F-E92B-DC4C-8BF0-A3E1B5948664}" name="32/32/2" totalsRowFunction="average" dataDxfId="49" totalsRowDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{3A5DB260-BC51-9943-9AA6-EF26448D4AB0}" name="Table121417" displayName="Table121417" ref="C61:F72" totalsRowCount="1" headerRowDxfId="73" dataDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{3A5DB260-BC51-9943-9AA6-EF26448D4AB0}" name="Table121417" displayName="Table121417" ref="C61:F72" totalsRowCount="1" headerRowDxfId="47" dataDxfId="46">
   <autoFilter ref="C61:F71" xr:uid="{77973C46-8BAA-9E42-9CF9-1BC781EFFEBC}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4700,19 +6006,19 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{611F1749-0588-F848-9620-3D32DE58D012}" name="1" totalsRowFunction="custom" dataDxfId="71" totalsRowDxfId="67">
+    <tableColumn id="1" xr3:uid="{611F1749-0588-F848-9620-3D32DE58D012}" name="1" totalsRowFunction="custom" dataDxfId="45" totalsRowDxfId="44">
       <totalsRowFormula>AVERAGE(Table121417[1])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5C8112FE-A4B8-2842-B70E-44A2DC4E2C86}" name="2" totalsRowFunction="average" dataDxfId="70" totalsRowDxfId="66"/>
-    <tableColumn id="3" xr3:uid="{4BB710EE-2F6B-104C-91C2-4D5DE8B5EA8D}" name="4" totalsRowFunction="average" dataDxfId="69" totalsRowDxfId="65"/>
-    <tableColumn id="4" xr3:uid="{A0144014-194E-4444-8B54-6D61F558C222}" name="8" totalsRowFunction="average" dataDxfId="68" totalsRowDxfId="64"/>
+    <tableColumn id="2" xr3:uid="{5C8112FE-A4B8-2842-B70E-44A2DC4E2C86}" name="2" totalsRowFunction="average" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{4BB710EE-2F6B-104C-91C2-4D5DE8B5EA8D}" name="4" totalsRowFunction="average" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{A0144014-194E-4444-8B54-6D61F558C222}" name="8" totalsRowFunction="average" dataDxfId="39" totalsRowDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{31496C44-A2F7-6046-A581-DE00E1A64495}" name="Table12141718" displayName="Table12141718" ref="L61:O72" totalsRowCount="1" headerRowDxfId="63" dataDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{31496C44-A2F7-6046-A581-DE00E1A64495}" name="Table12141718" displayName="Table12141718" ref="L61:O72" totalsRowCount="1" headerRowDxfId="37" dataDxfId="36">
   <autoFilter ref="L61:O71" xr:uid="{2A271704-5B21-F64E-8049-792EF620B77A}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4720,19 +6026,19 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D743CB9F-8265-124F-92C6-6757D444A101}" name="1" totalsRowFunction="custom" dataDxfId="60" totalsRowDxfId="61">
+    <tableColumn id="1" xr3:uid="{D743CB9F-8265-124F-92C6-6757D444A101}" name="1" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="34">
       <totalsRowFormula>AVERAGE(Table12141718[1])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5C8613A6-D77C-1E41-8FFD-A8DB9B432EFA}" name="2" totalsRowFunction="average" dataDxfId="58" totalsRowDxfId="59"/>
-    <tableColumn id="3" xr3:uid="{844C3824-E977-A14C-8C1A-147CFABDF145}" name="4" totalsRowFunction="average" dataDxfId="56" totalsRowDxfId="57"/>
-    <tableColumn id="4" xr3:uid="{245E9196-FB1E-2B4A-926B-2633671BC3A4}" name="8" totalsRowFunction="average" dataDxfId="54" totalsRowDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{5C8613A6-D77C-1E41-8FFD-A8DB9B432EFA}" name="2" totalsRowFunction="average" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{844C3824-E977-A14C-8C1A-147CFABDF145}" name="4" totalsRowFunction="average" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{245E9196-FB1E-2B4A-926B-2633671BC3A4}" name="8" totalsRowFunction="average" dataDxfId="29" totalsRowDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{D5DB36BD-3777-BD47-B388-C694D27FBE74}" name="Table12141519" displayName="Table12141519" ref="C87:H98" totalsRowCount="1" headerRowDxfId="53" dataDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{D5DB36BD-3777-BD47-B388-C694D27FBE74}" name="Table12141519" displayName="Table12141519" ref="C87:H98" totalsRowCount="1" headerRowDxfId="13" dataDxfId="27">
   <autoFilter ref="C87:H97" xr:uid="{1F757434-E3E5-594B-8FFA-2545970AF61F}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4742,21 +6048,21 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{9E17C061-277B-7145-AC08-E3828B5A8FB5}" name="1" totalsRowFunction="custom" dataDxfId="50" totalsRowDxfId="51">
-      <totalsRowFormula>AVERAGE(Table12141519[1])</totalsRowFormula>
+    <tableColumn id="1" xr3:uid="{9E17C061-277B-7145-AC08-E3828B5A8FB5}" name="56/1/2" totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="12">
+      <totalsRowFormula>AVERAGE(Table12141519[56/1/2])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{49DD9B33-6A59-EC46-9C7E-E574A972BCE4}" name="2" totalsRowFunction="average" dataDxfId="48" totalsRowDxfId="49"/>
-    <tableColumn id="3" xr3:uid="{7C11F312-D5FE-DE47-9FE3-98A59213BB44}" name="4" totalsRowFunction="average" dataDxfId="46" totalsRowDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{505390BD-3EED-7C4E-811B-893A241116FD}" name="8" totalsRowFunction="average" dataDxfId="44" totalsRowDxfId="45"/>
-    <tableColumn id="6" xr3:uid="{3B602D41-421B-204B-AF4D-3524607F2B3A}" name="16" totalsRowFunction="average" dataDxfId="42" totalsRowDxfId="43"/>
-    <tableColumn id="7" xr3:uid="{56545EED-A799-1045-ACA1-22CCA3BB785E}" name="32" totalsRowFunction="average" dataDxfId="40" totalsRowDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{49DD9B33-6A59-EC46-9C7E-E574A972BCE4}" name="112/2/4" totalsRowFunction="average" dataDxfId="25" totalsRowDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{7C11F312-D5FE-DE47-9FE3-98A59213BB44}" name="224/4/8" totalsRowFunction="average" dataDxfId="24" totalsRowDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{505390BD-3EED-7C4E-811B-893A241116FD}" name="448/8/16" totalsRowFunction="average" dataDxfId="23" totalsRowDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{3B602D41-421B-204B-AF4D-3524607F2B3A}" name="896/16/32" totalsRowFunction="average" dataDxfId="22" totalsRowDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{56545EED-A799-1045-ACA1-22CCA3BB785E}" name="1792/32/64" totalsRowFunction="average" dataDxfId="21" totalsRowDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{6588BB5D-67F0-BB43-9F21-59AFA57E8AF4}" name="Table1214151620" displayName="Table1214151620" ref="L87:Q98" totalsRowCount="1" headerRowDxfId="39" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{6588BB5D-67F0-BB43-9F21-59AFA57E8AF4}" name="Table1214151620" displayName="Table1214151620" ref="L87:Q98" totalsRowCount="1" headerRowDxfId="6" dataDxfId="20">
   <autoFilter ref="L87:Q97" xr:uid="{5512B521-6B77-F843-A5B4-F0AB0FB6DFB5}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4766,14 +6072,14 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{DB504DAF-52D8-1649-87BC-A7AB49A17859}" name="1" totalsRowFunction="custom" dataDxfId="36" totalsRowDxfId="37">
-      <totalsRowFormula>AVERAGE(Table1214151620[1])</totalsRowFormula>
+    <tableColumn id="1" xr3:uid="{DB504DAF-52D8-1649-87BC-A7AB49A17859}" name="56/1/2" totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="5">
+      <totalsRowFormula>AVERAGE(Table1214151620[56/1/2])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{EC6E11B1-7660-A14C-98A7-F5546CF00337}" name="2" totalsRowFunction="average" dataDxfId="34" totalsRowDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{209F27B7-05A6-E84B-99C5-22633169F39F}" name="4" totalsRowFunction="average" dataDxfId="32" totalsRowDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{8A07B38D-10AE-B547-8DB0-B10F4A88768B}" name="8" totalsRowFunction="average" dataDxfId="30" totalsRowDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{E94668A0-46D9-B345-87E9-B76EB6E2386B}" name="16" totalsRowFunction="average" dataDxfId="28" totalsRowDxfId="29"/>
-    <tableColumn id="7" xr3:uid="{7AC8FB38-E3D6-9749-97B8-32BB3B5174B0}" name="32" totalsRowFunction="average" dataDxfId="26" totalsRowDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{EC6E11B1-7660-A14C-98A7-F5546CF00337}" name="112/2/4" totalsRowFunction="average" dataDxfId="18" totalsRowDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{209F27B7-05A6-E84B-99C5-22633169F39F}" name="224/4/8" totalsRowFunction="average" dataDxfId="17" totalsRowDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{8A07B38D-10AE-B547-8DB0-B10F4A88768B}" name="448/8/16" totalsRowFunction="average" dataDxfId="16" totalsRowDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{E94668A0-46D9-B345-87E9-B76EB6E2386B}" name="896/16/32" totalsRowFunction="average" dataDxfId="15" totalsRowDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{7AC8FB38-E3D6-9749-97B8-32BB3B5174B0}" name="1792/32/64" totalsRowFunction="average" dataDxfId="14" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -5078,8 +6384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CACD4666-87E2-F84B-9806-2702F4658363}">
   <dimension ref="A1:AG99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="W67" sqref="W67"/>
+    <sheetView tabSelected="1" topLeftCell="O81" workbookViewId="0">
+      <selection activeCell="I116" sqref="I116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5098,33 +6404,33 @@
       <c r="D1" s="2"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>9</v>
+      <c r="C8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="4">
@@ -5139,24 +6445,24 @@
       <c r="F9" s="4">
         <v>100.26</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="L9" s="7">
+      <c r="L9" s="6">
         <v>102.15</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M9" s="6">
         <v>102.55</v>
       </c>
-      <c r="N9" s="7">
+      <c r="N9" s="6">
         <v>104.34</v>
       </c>
-      <c r="O9" s="7">
+      <c r="O9" s="6">
         <v>107.35</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B10" s="5"/>
+      <c r="B10" s="9"/>
       <c r="C10" s="4">
         <v>100.1</v>
       </c>
@@ -5169,22 +6475,22 @@
       <c r="F10" s="4">
         <v>100.25</v>
       </c>
-      <c r="K10" s="5"/>
-      <c r="L10" s="7">
+      <c r="K10" s="9"/>
+      <c r="L10" s="6">
         <v>102.34</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M10" s="6">
         <v>103</v>
       </c>
-      <c r="N10" s="7">
+      <c r="N10" s="6">
         <v>104.5</v>
       </c>
-      <c r="O10" s="7">
+      <c r="O10" s="6">
         <v>106.64</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B11" s="5"/>
+      <c r="B11" s="9"/>
       <c r="C11" s="4">
         <v>100.09</v>
       </c>
@@ -5197,22 +6503,22 @@
       <c r="F11" s="4">
         <v>100.25</v>
       </c>
-      <c r="K11" s="5"/>
-      <c r="L11" s="7">
+      <c r="K11" s="9"/>
+      <c r="L11" s="6">
         <v>102.3</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M11" s="6">
         <v>102.85</v>
       </c>
-      <c r="N11" s="7">
+      <c r="N11" s="6">
         <v>104.5</v>
       </c>
-      <c r="O11" s="7">
+      <c r="O11" s="6">
         <v>107.61</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B12" s="5"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="4">
         <v>100.02</v>
       </c>
@@ -5225,22 +6531,22 @@
       <c r="F12" s="4">
         <v>100.14</v>
       </c>
-      <c r="K12" s="5"/>
-      <c r="L12" s="7">
+      <c r="K12" s="9"/>
+      <c r="L12" s="6">
         <v>102.17</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="6">
         <v>103.24</v>
       </c>
-      <c r="N12" s="7">
+      <c r="N12" s="6">
         <v>104.57</v>
       </c>
-      <c r="O12" s="7">
+      <c r="O12" s="6">
         <v>107.61</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B13" s="5"/>
+      <c r="B13" s="9"/>
       <c r="C13" s="4">
         <v>100.12</v>
       </c>
@@ -5253,22 +6559,22 @@
       <c r="F13" s="4">
         <v>100.26</v>
       </c>
-      <c r="K13" s="5"/>
-      <c r="L13" s="7">
+      <c r="K13" s="9"/>
+      <c r="L13" s="6">
         <v>102.22</v>
       </c>
-      <c r="M13" s="7">
+      <c r="M13" s="6">
         <v>102.57</v>
       </c>
-      <c r="N13" s="7">
+      <c r="N13" s="6">
         <v>104.13</v>
       </c>
-      <c r="O13" s="7">
+      <c r="O13" s="6">
         <v>108.38</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B14" s="5"/>
+      <c r="B14" s="9"/>
       <c r="C14" s="4">
         <v>100.12</v>
       </c>
@@ -5281,22 +6587,22 @@
       <c r="F14" s="4">
         <v>100.24</v>
       </c>
-      <c r="K14" s="5"/>
-      <c r="L14" s="7">
+      <c r="K14" s="9"/>
+      <c r="L14" s="6">
         <v>101.97</v>
       </c>
-      <c r="M14" s="7">
+      <c r="M14" s="6">
         <v>102.87</v>
       </c>
-      <c r="N14" s="7">
+      <c r="N14" s="6">
         <v>105.08</v>
       </c>
-      <c r="O14" s="7">
+      <c r="O14" s="6">
         <v>106.85</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B15" s="5"/>
+      <c r="B15" s="9"/>
       <c r="C15" s="4">
         <v>100.12</v>
       </c>
@@ -5309,22 +6615,22 @@
       <c r="F15" s="4">
         <v>100.16</v>
       </c>
-      <c r="K15" s="5"/>
-      <c r="L15" s="7">
+      <c r="K15" s="9"/>
+      <c r="L15" s="6">
         <v>102.44</v>
       </c>
-      <c r="M15" s="7">
+      <c r="M15" s="6">
         <v>102.93</v>
       </c>
-      <c r="N15" s="7">
+      <c r="N15" s="6">
         <v>104.96</v>
       </c>
-      <c r="O15" s="7">
+      <c r="O15" s="6">
         <v>106.62</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B16" s="5"/>
+      <c r="B16" s="9"/>
       <c r="C16" s="4">
         <v>100.11</v>
       </c>
@@ -5337,22 +6643,22 @@
       <c r="F16" s="4">
         <v>100.33</v>
       </c>
-      <c r="K16" s="5"/>
-      <c r="L16" s="7">
+      <c r="K16" s="9"/>
+      <c r="L16" s="6">
         <v>102.22</v>
       </c>
-      <c r="M16" s="7">
+      <c r="M16" s="6">
         <v>103.1</v>
       </c>
-      <c r="N16" s="7">
+      <c r="N16" s="6">
         <v>104.34</v>
       </c>
-      <c r="O16" s="7">
+      <c r="O16" s="6">
         <v>107.31</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B17" s="5"/>
+      <c r="B17" s="9"/>
       <c r="C17" s="4">
         <v>100.08</v>
       </c>
@@ -5365,22 +6671,22 @@
       <c r="F17" s="4">
         <v>100.32</v>
       </c>
-      <c r="K17" s="5"/>
-      <c r="L17" s="7">
+      <c r="K17" s="9"/>
+      <c r="L17" s="6">
         <v>102.09</v>
       </c>
-      <c r="M17" s="7">
+      <c r="M17" s="6">
         <v>102.53</v>
       </c>
-      <c r="N17" s="7">
+      <c r="N17" s="6">
         <v>103.9</v>
       </c>
-      <c r="O17" s="7">
+      <c r="O17" s="6">
         <v>107.29</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B18" s="5"/>
+      <c r="B18" s="9"/>
       <c r="C18" s="4">
         <v>100.06</v>
       </c>
@@ -5393,97 +6699,97 @@
       <c r="F18" s="4">
         <v>100.2</v>
       </c>
-      <c r="K18" s="5"/>
-      <c r="L18" s="7">
+      <c r="K18" s="9"/>
+      <c r="L18" s="6">
         <v>102.14</v>
       </c>
-      <c r="M18" s="7">
+      <c r="M18" s="6">
         <v>102.75</v>
       </c>
-      <c r="N18" s="7">
+      <c r="N18" s="6">
         <v>104.73</v>
       </c>
-      <c r="O18" s="7">
+      <c r="O18" s="6">
         <v>106.65</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="7">
-        <f>AVERAGE(Table1214[1])</f>
+      <c r="C19" s="6">
+        <f>AVERAGE(Table1214[1/1/1])</f>
         <v>100.1</v>
       </c>
-      <c r="D19" s="7">
-        <f>SUBTOTAL(101,Table1214[2])</f>
+      <c r="D19" s="6">
+        <f>SUBTOTAL(101,Table1214[2/2/1])</f>
         <v>100.10799999999999</v>
       </c>
-      <c r="E19" s="7">
-        <f>SUBTOTAL(101,Table1214[4])</f>
+      <c r="E19" s="6">
+        <f>SUBTOTAL(101,Table1214[4/4/1])</f>
         <v>100.175</v>
       </c>
-      <c r="F19" s="7">
-        <f>SUBTOTAL(101,Table1214[8])</f>
+      <c r="F19" s="6">
+        <f>SUBTOTAL(101,Table1214[8/8/1])</f>
         <v>100.24100000000001</v>
       </c>
-      <c r="K19" s="6" t="s">
+      <c r="K19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L19" s="7">
-        <f>AVERAGE(Table12[1])</f>
+      <c r="L19" s="6">
+        <f>AVERAGE(Table12[1/1/1])</f>
         <v>102.20400000000002</v>
       </c>
-      <c r="M19" s="7">
-        <f>SUBTOTAL(101,Table12[2])</f>
+      <c r="M19" s="6">
+        <f>SUBTOTAL(101,Table12[2/2/1])</f>
         <v>102.83899999999998</v>
       </c>
-      <c r="N19" s="7">
-        <f>SUBTOTAL(101,Table12[4])</f>
+      <c r="N19" s="6">
+        <f>SUBTOTAL(101,Table12[4/4/1])</f>
         <v>104.505</v>
       </c>
-      <c r="O19" s="7">
-        <f>SUBTOTAL(101,Table12[8])</f>
+      <c r="O19" s="6">
+        <f>SUBTOTAL(101,Table12[8/8/1])</f>
         <v>107.23100000000002</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="7">
         <f>STDEV(C9:C18)</f>
         <v>4.2426406871195574E-2</v>
       </c>
-      <c r="D20" s="8">
-        <f t="shared" ref="D20:F20" si="0">STDEV(D9:D18)</f>
+      <c r="D20" s="7">
+        <f>STDEV(D9:D18)</f>
         <v>3.6147844564603231E-2</v>
       </c>
-      <c r="E20" s="8">
-        <f t="shared" si="0"/>
+      <c r="E20" s="7">
+        <f>STDEV(E9:E18)</f>
         <v>7.7064186811314231E-2</v>
       </c>
-      <c r="F20" s="8">
-        <f t="shared" si="0"/>
+      <c r="F20" s="7">
+        <f>STDEV(F9:F18)</f>
         <v>6.1000910740012924E-2</v>
       </c>
-      <c r="K20" s="6" t="s">
+      <c r="K20" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L20" s="8">
+      <c r="L20" s="7">
         <f>STDEV(L9:L18)</f>
         <v>0.13326664999166069</v>
       </c>
-      <c r="M20" s="8">
-        <f t="shared" ref="M20:O20" si="1">STDEV(M9:M18)</f>
+      <c r="M20" s="7">
+        <f>STDEV(M9:M18)</f>
         <v>0.24117536266284631</v>
       </c>
-      <c r="N20" s="8">
-        <f t="shared" si="1"/>
+      <c r="N20" s="7">
+        <f>STDEV(N9:N18)</f>
         <v>0.35802700084397537</v>
       </c>
-      <c r="O20" s="8">
-        <f t="shared" si="1"/>
+      <c r="O20" s="7">
+        <f>STDEV(O9:O18)</f>
         <v>0.56141586883323447</v>
       </c>
     </row>
@@ -5508,41 +6814,41 @@
       <c r="AG34" s="4"/>
     </row>
     <row r="35" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="C35" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G35" s="1" t="s">
+      <c r="C35" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H35" s="1" t="s">
+      <c r="D35" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="L35" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N35" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="O35" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P35" s="1" t="s">
+      <c r="E35" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L35" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="Q35" s="1" t="s">
+      <c r="M35" s="8" t="s">
         <v>13</v>
+      </c>
+      <c r="N35" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="O35" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="P35" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q35" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="X35" s="4"/>
       <c r="Y35" s="4"/>
@@ -5556,7 +6862,7 @@
       <c r="AG35" s="4"/>
     </row>
     <row r="36" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C36" s="4">
@@ -5577,7 +6883,7 @@
       <c r="H36" s="4">
         <v>104.24</v>
       </c>
-      <c r="K36" s="5" t="s">
+      <c r="K36" s="9" t="s">
         <v>1</v>
       </c>
       <c r="L36" s="4">
@@ -5610,7 +6916,7 @@
       <c r="AG36" s="4"/>
     </row>
     <row r="37" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B37" s="5"/>
+      <c r="B37" s="9"/>
       <c r="C37" s="4">
         <v>101.24</v>
       </c>
@@ -5629,7 +6935,7 @@
       <c r="H37" s="4">
         <v>102.83</v>
       </c>
-      <c r="K37" s="5"/>
+      <c r="K37" s="9"/>
       <c r="L37" s="4">
         <v>101.63</v>
       </c>
@@ -5660,7 +6966,7 @@
       <c r="AG37" s="4"/>
     </row>
     <row r="38" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B38" s="5"/>
+      <c r="B38" s="9"/>
       <c r="C38" s="4">
         <v>100.8</v>
       </c>
@@ -5679,7 +6985,7 @@
       <c r="H38" s="4">
         <v>103.89</v>
       </c>
-      <c r="K38" s="5"/>
+      <c r="K38" s="9"/>
       <c r="L38" s="4">
         <v>101.38</v>
       </c>
@@ -5710,7 +7016,7 @@
       <c r="AG38" s="4"/>
     </row>
     <row r="39" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B39" s="5"/>
+      <c r="B39" s="9"/>
       <c r="C39" s="4">
         <v>101.21</v>
       </c>
@@ -5729,7 +7035,7 @@
       <c r="H39" s="4">
         <v>102.88</v>
       </c>
-      <c r="K39" s="5"/>
+      <c r="K39" s="9"/>
       <c r="L39" s="4">
         <v>101.55</v>
       </c>
@@ -5760,7 +7066,7 @@
       <c r="AG39" s="4"/>
     </row>
     <row r="40" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B40" s="5"/>
+      <c r="B40" s="9"/>
       <c r="C40" s="4">
         <v>101.33</v>
       </c>
@@ -5779,7 +7085,7 @@
       <c r="H40" s="4">
         <v>104.92</v>
       </c>
-      <c r="K40" s="5"/>
+      <c r="K40" s="9"/>
       <c r="L40" s="4">
         <v>101.97</v>
       </c>
@@ -5800,7 +7106,7 @@
       </c>
     </row>
     <row r="41" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B41" s="5"/>
+      <c r="B41" s="9"/>
       <c r="C41" s="4">
         <v>100.78</v>
       </c>
@@ -5819,7 +7125,7 @@
       <c r="H41" s="4">
         <v>103.58</v>
       </c>
-      <c r="K41" s="5"/>
+      <c r="K41" s="9"/>
       <c r="L41" s="4">
         <v>101.44</v>
       </c>
@@ -5840,7 +7146,7 @@
       </c>
     </row>
     <row r="42" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B42" s="5"/>
+      <c r="B42" s="9"/>
       <c r="C42" s="4">
         <v>101.36</v>
       </c>
@@ -5859,7 +7165,7 @@
       <c r="H42" s="4">
         <v>102.9</v>
       </c>
-      <c r="K42" s="5"/>
+      <c r="K42" s="9"/>
       <c r="L42" s="4">
         <v>101.77</v>
       </c>
@@ -5880,7 +7186,7 @@
       </c>
     </row>
     <row r="43" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B43" s="5"/>
+      <c r="B43" s="9"/>
       <c r="C43" s="4">
         <v>101.1</v>
       </c>
@@ -5899,7 +7205,7 @@
       <c r="H43" s="4">
         <v>102.74</v>
       </c>
-      <c r="K43" s="5"/>
+      <c r="K43" s="9"/>
       <c r="L43" s="4">
         <v>101.49</v>
       </c>
@@ -5920,7 +7226,7 @@
       </c>
     </row>
     <row r="44" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B44" s="5"/>
+      <c r="B44" s="9"/>
       <c r="C44" s="4">
         <v>101.11</v>
       </c>
@@ -5939,7 +7245,7 @@
       <c r="H44" s="4">
         <v>103.2</v>
       </c>
-      <c r="K44" s="5"/>
+      <c r="K44" s="9"/>
       <c r="L44" s="4">
         <v>101.48</v>
       </c>
@@ -5960,7 +7266,7 @@
       </c>
     </row>
     <row r="45" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B45" s="5"/>
+      <c r="B45" s="9"/>
       <c r="C45" s="4">
         <v>101.22</v>
       </c>
@@ -5979,7 +7285,7 @@
       <c r="H45" s="4">
         <v>104.77</v>
       </c>
-      <c r="K45" s="5"/>
+      <c r="K45" s="9"/>
       <c r="L45" s="4">
         <v>101.42</v>
       </c>
@@ -6000,114 +7306,114 @@
       </c>
     </row>
     <row r="46" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C46" s="7">
-        <f>AVERAGE(Table121415[1])</f>
+      <c r="C46" s="6">
+        <f>AVERAGE(Table121415[1/1/1])</f>
         <v>101.12700000000001</v>
       </c>
-      <c r="D46" s="7">
-        <f>SUBTOTAL(101,Table121415[2])</f>
+      <c r="D46" s="6">
+        <f>SUBTOTAL(101,Table121415[2/2/1])</f>
         <v>101.096</v>
       </c>
-      <c r="E46" s="7">
-        <f>SUBTOTAL(101,Table121415[4])</f>
+      <c r="E46" s="6">
+        <f>SUBTOTAL(101,Table121415[4/4/1])</f>
         <v>101.161</v>
       </c>
-      <c r="F46" s="7">
-        <f>SUBTOTAL(101,Table121415[8])</f>
+      <c r="F46" s="6">
+        <f>SUBTOTAL(101,Table121415[8/8/1])</f>
         <v>101.357</v>
       </c>
-      <c r="G46" s="7">
-        <f>SUBTOTAL(101,Table121415[16])</f>
+      <c r="G46" s="6">
+        <f>SUBTOTAL(101,Table121415[16/16/1])</f>
         <v>101.63000000000001</v>
       </c>
-      <c r="H46" s="7">
-        <f>SUBTOTAL(101,Table121415[32])</f>
+      <c r="H46" s="6">
+        <f>SUBTOTAL(101,Table121415[32/32/2])</f>
         <v>103.595</v>
       </c>
-      <c r="K46" s="6" t="s">
+      <c r="K46" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L46" s="7">
-        <f>AVERAGE(Table12141516[1])</f>
+      <c r="L46" s="6">
+        <f>AVERAGE(Table12141516[1/1/1])</f>
         <v>101.52499999999999</v>
       </c>
-      <c r="M46" s="7">
-        <f>SUBTOTAL(101,Table12141516[2])</f>
+      <c r="M46" s="6">
+        <f>SUBTOTAL(101,Table12141516[2/2/1])</f>
         <v>101.596</v>
       </c>
-      <c r="N46" s="7">
-        <f>SUBTOTAL(101,Table12141516[4])</f>
+      <c r="N46" s="6">
+        <f>SUBTOTAL(101,Table12141516[4/4/1])</f>
         <v>101.502</v>
       </c>
-      <c r="O46" s="7">
-        <f>SUBTOTAL(101,Table12141516[8])</f>
+      <c r="O46" s="6">
+        <f>SUBTOTAL(101,Table12141516[8/8/1])</f>
         <v>101.63400000000001</v>
       </c>
-      <c r="P46" s="7">
-        <f>SUBTOTAL(101,Table12141516[16])</f>
+      <c r="P46" s="6">
+        <f>SUBTOTAL(101,Table12141516[16/16/1])</f>
         <v>102.089</v>
       </c>
-      <c r="Q46" s="7">
-        <f>SUBTOTAL(101,Table12141516[32])</f>
+      <c r="Q46" s="6">
+        <f>SUBTOTAL(101,Table12141516[32/32/2])</f>
         <v>103.88500000000002</v>
       </c>
     </row>
     <row r="47" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C47" s="8">
+      <c r="C47" s="7">
         <f>STDEV(C36:C45)</f>
         <v>0.19782427668121072</v>
       </c>
-      <c r="D47" s="8">
-        <f t="shared" ref="D47:H47" si="2">STDEV(D36:D45)</f>
+      <c r="D47" s="7">
+        <f t="shared" ref="D47:H47" si="0">STDEV(D36:D45)</f>
         <v>0.25180239165751317</v>
       </c>
-      <c r="E47" s="8">
-        <f t="shared" si="2"/>
+      <c r="E47" s="7">
+        <f t="shared" si="0"/>
         <v>0.21163123062954953</v>
       </c>
-      <c r="F47" s="8">
-        <f t="shared" si="2"/>
+      <c r="F47" s="7">
+        <f t="shared" si="0"/>
         <v>0.30335347918448979</v>
       </c>
-      <c r="G47" s="8">
-        <f t="shared" si="2"/>
+      <c r="G47" s="7">
+        <f t="shared" si="0"/>
         <v>0.2171021265057842</v>
       </c>
-      <c r="H47" s="8">
-        <f t="shared" si="2"/>
+      <c r="H47" s="7">
+        <f t="shared" si="0"/>
         <v>0.82368076340290941</v>
       </c>
-      <c r="K47" s="6" t="s">
+      <c r="K47" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L47" s="8">
+      <c r="L47" s="7">
         <f>STDEV(L36:L45)</f>
         <v>0.23003622903070281</v>
       </c>
-      <c r="M47" s="8">
-        <f t="shared" ref="M47:Q47" si="3">STDEV(M36:M45)</f>
+      <c r="M47" s="7">
+        <f t="shared" ref="M47:Q47" si="1">STDEV(M36:M45)</f>
         <v>0.26315183618756754</v>
       </c>
-      <c r="N47" s="8">
-        <f t="shared" si="3"/>
+      <c r="N47" s="7">
+        <f t="shared" si="1"/>
         <v>0.30117547487580559</v>
       </c>
-      <c r="O47" s="8">
-        <f t="shared" si="3"/>
+      <c r="O47" s="7">
+        <f t="shared" si="1"/>
         <v>0.3333066655999149</v>
       </c>
-      <c r="P47" s="8">
-        <f t="shared" si="3"/>
+      <c r="P47" s="7">
+        <f t="shared" si="1"/>
         <v>0.38524018481980676</v>
       </c>
-      <c r="Q47" s="8">
-        <f t="shared" si="3"/>
+      <c r="Q47" s="7">
+        <f t="shared" si="1"/>
         <v>1.5162032258975791</v>
       </c>
     </row>
@@ -6145,7 +7451,7 @@
       </c>
     </row>
     <row r="62" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C62" s="4">
@@ -6160,7 +7466,7 @@
       <c r="F62" s="4">
         <v>0</v>
       </c>
-      <c r="K62" s="5" t="s">
+      <c r="K62" s="9" t="s">
         <v>1</v>
       </c>
       <c r="L62" s="4">
@@ -6187,7 +7493,7 @@
       <c r="AC62" s="4"/>
     </row>
     <row r="63" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B63" s="5"/>
+      <c r="B63" s="9"/>
       <c r="C63" s="4">
         <v>0</v>
       </c>
@@ -6200,7 +7506,7 @@
       <c r="F63" s="4">
         <v>0</v>
       </c>
-      <c r="K63" s="5"/>
+      <c r="K63" s="9"/>
       <c r="L63" s="4">
         <v>0</v>
       </c>
@@ -6225,7 +7531,7 @@
       <c r="AC63" s="4"/>
     </row>
     <row r="64" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B64" s="5"/>
+      <c r="B64" s="9"/>
       <c r="C64" s="4">
         <v>0</v>
       </c>
@@ -6238,7 +7544,7 @@
       <c r="F64" s="4">
         <v>0</v>
       </c>
-      <c r="K64" s="5"/>
+      <c r="K64" s="9"/>
       <c r="L64" s="4">
         <v>0</v>
       </c>
@@ -6263,7 +7569,7 @@
       <c r="AC64" s="4"/>
     </row>
     <row r="65" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B65" s="5"/>
+      <c r="B65" s="9"/>
       <c r="C65" s="4">
         <v>0</v>
       </c>
@@ -6276,7 +7582,7 @@
       <c r="F65" s="4">
         <v>0</v>
       </c>
-      <c r="K65" s="5"/>
+      <c r="K65" s="9"/>
       <c r="L65" s="4">
         <v>0</v>
       </c>
@@ -6301,7 +7607,7 @@
       <c r="AC65" s="4"/>
     </row>
     <row r="66" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B66" s="5"/>
+      <c r="B66" s="9"/>
       <c r="C66" s="4">
         <v>0</v>
       </c>
@@ -6314,7 +7620,7 @@
       <c r="F66" s="4">
         <v>0</v>
       </c>
-      <c r="K66" s="5"/>
+      <c r="K66" s="9"/>
       <c r="L66" s="4">
         <v>0</v>
       </c>
@@ -6339,7 +7645,7 @@
       <c r="AC66" s="4"/>
     </row>
     <row r="67" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B67" s="5"/>
+      <c r="B67" s="9"/>
       <c r="C67" s="4">
         <v>0</v>
       </c>
@@ -6352,7 +7658,7 @@
       <c r="F67" s="4">
         <v>0</v>
       </c>
-      <c r="K67" s="5"/>
+      <c r="K67" s="9"/>
       <c r="L67" s="4">
         <v>0</v>
       </c>
@@ -6377,7 +7683,7 @@
       <c r="AC67" s="4"/>
     </row>
     <row r="68" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B68" s="5"/>
+      <c r="B68" s="9"/>
       <c r="C68" s="4">
         <v>0</v>
       </c>
@@ -6390,7 +7696,7 @@
       <c r="F68" s="4">
         <v>0</v>
       </c>
-      <c r="K68" s="5"/>
+      <c r="K68" s="9"/>
       <c r="L68" s="4">
         <v>0</v>
       </c>
@@ -6405,7 +7711,7 @@
       </c>
     </row>
     <row r="69" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B69" s="5"/>
+      <c r="B69" s="9"/>
       <c r="C69" s="4">
         <v>0</v>
       </c>
@@ -6418,7 +7724,7 @@
       <c r="F69" s="4">
         <v>0</v>
       </c>
-      <c r="K69" s="5"/>
+      <c r="K69" s="9"/>
       <c r="L69" s="4">
         <v>0</v>
       </c>
@@ -6433,7 +7739,7 @@
       </c>
     </row>
     <row r="70" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B70" s="5"/>
+      <c r="B70" s="9"/>
       <c r="C70" s="4">
         <v>0</v>
       </c>
@@ -6446,7 +7752,7 @@
       <c r="F70" s="4">
         <v>0</v>
       </c>
-      <c r="K70" s="5"/>
+      <c r="K70" s="9"/>
       <c r="L70" s="4">
         <v>0</v>
       </c>
@@ -6461,7 +7767,7 @@
       </c>
     </row>
     <row r="71" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B71" s="5"/>
+      <c r="B71" s="9"/>
       <c r="C71" s="4">
         <v>0</v>
       </c>
@@ -6474,7 +7780,7 @@
       <c r="F71" s="4">
         <v>0</v>
       </c>
-      <c r="K71" s="5"/>
+      <c r="K71" s="9"/>
       <c r="L71" s="4">
         <v>0</v>
       </c>
@@ -6489,82 +7795,82 @@
       </c>
     </row>
     <row r="72" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B72" s="6" t="s">
+      <c r="B72" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C72" s="7">
+      <c r="C72" s="6">
         <f>AVERAGE(Table121417[1])</f>
         <v>0</v>
       </c>
-      <c r="D72" s="7">
+      <c r="D72" s="6">
         <f>SUBTOTAL(101,Table121417[2])</f>
         <v>0</v>
       </c>
-      <c r="E72" s="7">
+      <c r="E72" s="6">
         <f>SUBTOTAL(101,Table121417[4])</f>
         <v>0</v>
       </c>
-      <c r="F72" s="7">
+      <c r="F72" s="6">
         <f>SUBTOTAL(101,Table121417[8])</f>
         <v>0</v>
       </c>
-      <c r="K72" s="6" t="s">
+      <c r="K72" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L72" s="7">
+      <c r="L72" s="6">
         <f>AVERAGE(Table12141718[1])</f>
         <v>0</v>
       </c>
-      <c r="M72" s="7">
+      <c r="M72" s="6">
         <f>SUBTOTAL(101,Table12141718[2])</f>
         <v>0</v>
       </c>
-      <c r="N72" s="7">
+      <c r="N72" s="6">
         <f>SUBTOTAL(101,Table12141718[4])</f>
         <v>0</v>
       </c>
-      <c r="O72" s="7">
+      <c r="O72" s="6">
         <f>SUBTOTAL(101,Table12141718[8])</f>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B73" s="6" t="s">
+      <c r="B73" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C73" s="8">
+      <c r="C73" s="7">
         <f>STDEV(C62:C71)</f>
         <v>0</v>
       </c>
-      <c r="D73" s="8">
-        <f t="shared" ref="D73:F73" si="4">STDEV(D62:D71)</f>
-        <v>0</v>
-      </c>
-      <c r="E73" s="8">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F73" s="8">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="K73" s="6" t="s">
+      <c r="D73" s="7">
+        <f t="shared" ref="D73:F73" si="2">STDEV(D62:D71)</f>
+        <v>0</v>
+      </c>
+      <c r="E73" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F73" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K73" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L73" s="8">
+      <c r="L73" s="7">
         <f>STDEV(L62:L71)</f>
         <v>0</v>
       </c>
-      <c r="M73" s="8">
-        <f t="shared" ref="M73:O73" si="5">STDEV(M62:M71)</f>
-        <v>0</v>
-      </c>
-      <c r="N73" s="8">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O73" s="8">
-        <f t="shared" si="5"/>
+      <c r="M73" s="7">
+        <f t="shared" ref="M73:O73" si="3">STDEV(M62:M71)</f>
+        <v>0</v>
+      </c>
+      <c r="N73" s="7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O73" s="7">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -6576,45 +7882,45 @@
       <c r="C80" s="2"/>
     </row>
     <row r="87" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="C87" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G87" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H87" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L87" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M87" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="N87" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="O87" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="P87" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q87" s="1" t="s">
-        <v>13</v>
+      <c r="C87" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E87" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F87" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G87" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H87" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="L87" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M87" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N87" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="O87" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="P87" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q87" s="8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="88" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B88" s="5" t="s">
+      <c r="B88" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C88" s="4">
@@ -6635,7 +7941,7 @@
       <c r="H88" s="4">
         <v>0</v>
       </c>
-      <c r="K88" s="5" t="s">
+      <c r="K88" s="9" t="s">
         <v>1</v>
       </c>
       <c r="L88" s="4">
@@ -6658,7 +7964,7 @@
       </c>
     </row>
     <row r="89" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B89" s="5"/>
+      <c r="B89" s="9"/>
       <c r="C89" s="4">
         <v>0</v>
       </c>
@@ -6677,7 +7983,7 @@
       <c r="H89" s="4">
         <v>0</v>
       </c>
-      <c r="K89" s="5"/>
+      <c r="K89" s="9"/>
       <c r="L89" s="4">
         <v>0</v>
       </c>
@@ -6698,7 +8004,7 @@
       </c>
     </row>
     <row r="90" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B90" s="5"/>
+      <c r="B90" s="9"/>
       <c r="C90" s="4">
         <v>0</v>
       </c>
@@ -6717,7 +8023,7 @@
       <c r="H90" s="4">
         <v>0</v>
       </c>
-      <c r="K90" s="5"/>
+      <c r="K90" s="9"/>
       <c r="L90" s="4">
         <v>0</v>
       </c>
@@ -6738,7 +8044,7 @@
       </c>
     </row>
     <row r="91" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B91" s="5"/>
+      <c r="B91" s="9"/>
       <c r="C91" s="4">
         <v>0</v>
       </c>
@@ -6757,7 +8063,7 @@
       <c r="H91" s="4">
         <v>0</v>
       </c>
-      <c r="K91" s="5"/>
+      <c r="K91" s="9"/>
       <c r="L91" s="4">
         <v>0</v>
       </c>
@@ -6778,7 +8084,7 @@
       </c>
     </row>
     <row r="92" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B92" s="5"/>
+      <c r="B92" s="9"/>
       <c r="C92" s="4">
         <v>0</v>
       </c>
@@ -6797,7 +8103,7 @@
       <c r="H92" s="4">
         <v>0</v>
       </c>
-      <c r="K92" s="5"/>
+      <c r="K92" s="9"/>
       <c r="L92" s="4">
         <v>0</v>
       </c>
@@ -6818,7 +8124,7 @@
       </c>
     </row>
     <row r="93" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B93" s="5"/>
+      <c r="B93" s="9"/>
       <c r="C93" s="4">
         <v>0</v>
       </c>
@@ -6837,7 +8143,7 @@
       <c r="H93" s="4">
         <v>0</v>
       </c>
-      <c r="K93" s="5"/>
+      <c r="K93" s="9"/>
       <c r="L93" s="4">
         <v>0</v>
       </c>
@@ -6858,7 +8164,7 @@
       </c>
     </row>
     <row r="94" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B94" s="5"/>
+      <c r="B94" s="9"/>
       <c r="C94" s="4">
         <v>0</v>
       </c>
@@ -6877,7 +8183,7 @@
       <c r="H94" s="4">
         <v>0</v>
       </c>
-      <c r="K94" s="5"/>
+      <c r="K94" s="9"/>
       <c r="L94" s="4">
         <v>0</v>
       </c>
@@ -6898,7 +8204,7 @@
       </c>
     </row>
     <row r="95" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B95" s="5"/>
+      <c r="B95" s="9"/>
       <c r="C95" s="4">
         <v>0</v>
       </c>
@@ -6917,7 +8223,7 @@
       <c r="H95" s="4">
         <v>0</v>
       </c>
-      <c r="K95" s="5"/>
+      <c r="K95" s="9"/>
       <c r="L95" s="4">
         <v>0</v>
       </c>
@@ -6938,7 +8244,7 @@
       </c>
     </row>
     <row r="96" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B96" s="5"/>
+      <c r="B96" s="9"/>
       <c r="C96" s="4">
         <v>0</v>
       </c>
@@ -6957,7 +8263,7 @@
       <c r="H96" s="4">
         <v>0</v>
       </c>
-      <c r="K96" s="5"/>
+      <c r="K96" s="9"/>
       <c r="L96" s="4">
         <v>0</v>
       </c>
@@ -6978,7 +8284,7 @@
       </c>
     </row>
     <row r="97" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B97" s="5"/>
+      <c r="B97" s="9"/>
       <c r="C97" s="4">
         <v>0</v>
       </c>
@@ -6997,7 +8303,7 @@
       <c r="H97" s="4">
         <v>0</v>
       </c>
-      <c r="K97" s="5"/>
+      <c r="K97" s="9"/>
       <c r="L97" s="4">
         <v>0</v>
       </c>
@@ -7018,114 +8324,114 @@
       </c>
     </row>
     <row r="98" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B98" s="6" t="s">
+      <c r="B98" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C98" s="7">
-        <f>AVERAGE(Table12141519[1])</f>
-        <v>0</v>
-      </c>
-      <c r="D98" s="7">
-        <f>SUBTOTAL(101,Table12141519[2])</f>
-        <v>0</v>
-      </c>
-      <c r="E98" s="7">
-        <f>SUBTOTAL(101,Table12141519[4])</f>
-        <v>0</v>
-      </c>
-      <c r="F98" s="7">
-        <f>SUBTOTAL(101,Table12141519[8])</f>
-        <v>0</v>
-      </c>
-      <c r="G98" s="7">
-        <f>SUBTOTAL(101,Table12141519[16])</f>
-        <v>0</v>
-      </c>
-      <c r="H98" s="7">
-        <f>SUBTOTAL(101,Table12141519[32])</f>
-        <v>0</v>
-      </c>
-      <c r="K98" s="6" t="s">
+      <c r="C98" s="6">
+        <f>AVERAGE(Table12141519[56/1/2])</f>
+        <v>0</v>
+      </c>
+      <c r="D98" s="6">
+        <f>SUBTOTAL(101,Table12141519[112/2/4])</f>
+        <v>0</v>
+      </c>
+      <c r="E98" s="6">
+        <f>SUBTOTAL(101,Table12141519[224/4/8])</f>
+        <v>0</v>
+      </c>
+      <c r="F98" s="6">
+        <f>SUBTOTAL(101,Table12141519[448/8/16])</f>
+        <v>0</v>
+      </c>
+      <c r="G98" s="6">
+        <f>SUBTOTAL(101,Table12141519[896/16/32])</f>
+        <v>0</v>
+      </c>
+      <c r="H98" s="6">
+        <f>SUBTOTAL(101,Table12141519[1792/32/64])</f>
+        <v>0</v>
+      </c>
+      <c r="K98" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L98" s="7">
-        <f>AVERAGE(Table1214151620[1])</f>
-        <v>0</v>
-      </c>
-      <c r="M98" s="7">
-        <f>SUBTOTAL(101,Table1214151620[2])</f>
-        <v>0</v>
-      </c>
-      <c r="N98" s="7">
-        <f>SUBTOTAL(101,Table1214151620[4])</f>
-        <v>0</v>
-      </c>
-      <c r="O98" s="7">
-        <f>SUBTOTAL(101,Table1214151620[8])</f>
-        <v>0</v>
-      </c>
-      <c r="P98" s="7">
-        <f>SUBTOTAL(101,Table1214151620[16])</f>
-        <v>0</v>
-      </c>
-      <c r="Q98" s="7">
-        <f>SUBTOTAL(101,Table1214151620[32])</f>
+      <c r="L98" s="6">
+        <f>AVERAGE(Table1214151620[56/1/2])</f>
+        <v>0</v>
+      </c>
+      <c r="M98" s="6">
+        <f>SUBTOTAL(101,Table1214151620[112/2/4])</f>
+        <v>0</v>
+      </c>
+      <c r="N98" s="6">
+        <f>SUBTOTAL(101,Table1214151620[224/4/8])</f>
+        <v>0</v>
+      </c>
+      <c r="O98" s="6">
+        <f>SUBTOTAL(101,Table1214151620[448/8/16])</f>
+        <v>0</v>
+      </c>
+      <c r="P98" s="6">
+        <f>SUBTOTAL(101,Table1214151620[896/16/32])</f>
+        <v>0</v>
+      </c>
+      <c r="Q98" s="6">
+        <f>SUBTOTAL(101,Table1214151620[1792/32/64])</f>
         <v>0</v>
       </c>
     </row>
     <row r="99" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B99" s="6" t="s">
+      <c r="B99" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C99" s="8">
+      <c r="C99" s="7">
         <f>STDEV(C88:C97)</f>
         <v>0</v>
       </c>
-      <c r="D99" s="8">
-        <f t="shared" ref="D99:H99" si="6">STDEV(D88:D97)</f>
-        <v>0</v>
-      </c>
-      <c r="E99" s="8">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="F99" s="8">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="G99" s="8">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="H99" s="8">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K99" s="6" t="s">
+      <c r="D99" s="7">
+        <f t="shared" ref="D99:H99" si="4">STDEV(D88:D97)</f>
+        <v>0</v>
+      </c>
+      <c r="E99" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F99" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G99" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H99" s="7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="K99" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L99" s="8">
+      <c r="L99" s="7">
         <f>STDEV(L88:L97)</f>
         <v>0</v>
       </c>
-      <c r="M99" s="8">
-        <f t="shared" ref="M99:Q99" si="7">STDEV(M88:M97)</f>
-        <v>0</v>
-      </c>
-      <c r="N99" s="8">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="O99" s="8">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="P99" s="8">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Q99" s="8">
-        <f t="shared" si="7"/>
+      <c r="M99" s="7">
+        <f t="shared" ref="M99:Q99" si="5">STDEV(M88:M97)</f>
+        <v>0</v>
+      </c>
+      <c r="N99" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O99" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P99" s="7">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="Q99" s="7">
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed Intel MPI container experiment results on Comet
</commit_message>
<xml_diff>
--- a/Containers/First experiments/results/results.xlsx
+++ b/Containers/First experiments/results/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karahbit/koubbe/Containers/First experiments/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB498FB-E018-3940-BE92-0C78D02BBD99}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AB56DF-C0DF-7842-835F-46A1717683CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{5C86F751-EA59-464C-941B-333EDFC81949}"/>
+    <workbookView xWindow="860" yWindow="460" windowWidth="37540" windowHeight="21140" xr2:uid="{5C86F751-EA59-464C-941B-333EDFC81949}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="29">
   <si>
     <t>non-containerized</t>
   </si>
@@ -110,6 +110,9 @@
   <si>
     <t>MPICH Hello World on Comet using Singularity</t>
   </si>
+  <si>
+    <t>Intel MPI Hello World on Comet using Singularity (fixed)</t>
+  </si>
 </sst>
 </file>
 
@@ -188,7 +191,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="128">
+  <dxfs count="148">
     <dxf>
       <font>
         <b val="0"/>
@@ -434,6 +437,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -509,7 +513,10 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -528,6 +535,10 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -606,10 +617,6 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -686,6 +693,24 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1130,10 +1155,336 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <font>
@@ -6321,6 +6672,758 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1700" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Intel MPI 18.1 Hello World on Comet using Singularity 3.5 (fixed)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1700">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>non-containerized</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$C$177:$F$177</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>0.6811885038502794</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.45668978043695629</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>8.752698694942266</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>9.0459171883108542</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$C$177:$F$177</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>0.6811885038502794</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.45668978043695629</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>8.752698694942266</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>9.0459171883108542</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$165:$F$165</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>48/1/2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>96/2/4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>192/4/8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>384/8/16</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$176:$F$176</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>4.6379999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.7809999999999988</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32.777000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>97.667999999999978</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3529-4C47-9CA1-E9D7AAA8A699}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>containerized</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$J$177:$M$177</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>1.9435523032724265</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.0469155754989139</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4.895857205615548</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>12.055468514790807</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$J$177:$M$177</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>1.9435523032724265</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.0469155754989139</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4.895857205615548</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>12.055468514790807</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$165:$F$165</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>48/1/2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>96/2/4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>192/4/8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>384/8/16</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$176:$M$176</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5.1280000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.548999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33.428000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>99.498999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3529-4C47-9CA1-E9D7AAA8A699}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1743758432"/>
+        <c:axId val="1766352896"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1743758432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>cores/tasks/nodes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1766352896"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1766352896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>TTX</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (seconds)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1743758432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -6521,6 +7624,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -8534,6 +9677,509 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -9192,14 +10838,14 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>135</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
       <xdr:row>156</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9226,11 +10872,49 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>161</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>182</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FD3AE78-02C8-1742-A1D2-5BE0B4664650}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{AB51CF61-79E3-FF4F-B384-F02243D3273A}" name="Table12" displayName="Table12" ref="L8:O19" totalsRowCount="1" headerRowDxfId="127" dataDxfId="126">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{AB51CF61-79E3-FF4F-B384-F02243D3273A}" name="Table12" displayName="Table12" ref="L8:O19" totalsRowCount="1" headerRowDxfId="147" dataDxfId="146">
   <autoFilter ref="L8:O18" xr:uid="{4157A701-19DE-9F43-9C32-34B7BD7CBED0}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -9238,19 +10922,19 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A2B04CA0-9DF0-5F41-B767-0E628D6F8EE7}" name="1/1/1" totalsRowFunction="custom" dataDxfId="125" totalsRowDxfId="124">
+    <tableColumn id="1" xr3:uid="{A2B04CA0-9DF0-5F41-B767-0E628D6F8EE7}" name="1/1/1" totalsRowFunction="custom" dataDxfId="145" totalsRowDxfId="144">
       <totalsRowFormula>AVERAGE(Table12[1/1/1])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{C90CC318-E4DA-9B40-A32D-3102841F0921}" name="2/2/1" totalsRowFunction="average" dataDxfId="123" totalsRowDxfId="122"/>
-    <tableColumn id="3" xr3:uid="{61A7C00A-F63D-C44A-AFA0-6B9EC0793A33}" name="4/4/1" totalsRowFunction="average" dataDxfId="121" totalsRowDxfId="120"/>
-    <tableColumn id="4" xr3:uid="{56012B1C-DD0E-0744-9080-C13899D5A44A}" name="8/8/1" totalsRowFunction="average" dataDxfId="119" totalsRowDxfId="118"/>
+    <tableColumn id="2" xr3:uid="{C90CC318-E4DA-9B40-A32D-3102841F0921}" name="2/2/1" totalsRowFunction="average" dataDxfId="143" totalsRowDxfId="142"/>
+    <tableColumn id="3" xr3:uid="{61A7C00A-F63D-C44A-AFA0-6B9EC0793A33}" name="4/4/1" totalsRowFunction="average" dataDxfId="141" totalsRowDxfId="140"/>
+    <tableColumn id="4" xr3:uid="{56012B1C-DD0E-0744-9080-C13899D5A44A}" name="8/8/1" totalsRowFunction="average" dataDxfId="139" totalsRowDxfId="138"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{52426DB4-14EA-2649-8CB2-1D2DAFDA3B15}" name="Table12141516205" displayName="Table12141516205" ref="J113:M124" totalsRowCount="1" headerRowDxfId="37" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{52426DB4-14EA-2649-8CB2-1D2DAFDA3B15}" name="Table12141516205" displayName="Table12141516205" ref="J113:M124" totalsRowCount="1" headerRowDxfId="49" dataDxfId="48">
   <autoFilter ref="J113:M123" xr:uid="{F034FC1F-3CF7-B942-B308-85E14F5AA64F}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -9258,19 +10942,19 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{B23176C4-4048-7E4C-93F7-48A12948FA7D}" name="48/1/2" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="34">
+    <tableColumn id="1" xr3:uid="{B23176C4-4048-7E4C-93F7-48A12948FA7D}" name="48/1/2" totalsRowFunction="custom" dataDxfId="47" totalsRowDxfId="46">
       <totalsRowFormula>AVERAGE(Table12141516205[48/1/2])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{A9911769-69F4-A741-BA92-8BC1FDB2B783}" name="96/2/4" totalsRowFunction="average" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{9AF887F1-C47A-B242-89FA-FF10EAAE3937}" name="192/4/8" totalsRowFunction="average" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{D8B4360F-298E-3248-9842-128248D56CBF}" name="384/8/16" totalsRowFunction="average" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{A9911769-69F4-A741-BA92-8BC1FDB2B783}" name="96/2/4" totalsRowFunction="average" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{9AF887F1-C47A-B242-89FA-FF10EAAE3937}" name="192/4/8" totalsRowFunction="average" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{D8B4360F-298E-3248-9842-128248D56CBF}" name="384/8/16" totalsRowFunction="average" dataDxfId="41" totalsRowDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0D9A6B2D-529B-7041-9E85-89062843DDC9}" name="Table1214151942" displayName="Table1214151942" ref="C139:F150" totalsRowCount="1" headerRowDxfId="27" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0D9A6B2D-529B-7041-9E85-89062843DDC9}" name="Table1214151942" displayName="Table1214151942" ref="C139:F150" totalsRowCount="1" headerRowDxfId="39" dataDxfId="38">
   <autoFilter ref="C139:F149" xr:uid="{5CC8DAB3-56BF-304B-8AA6-4ABCC8E25A47}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -9278,19 +10962,19 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{80FFCD29-7FFB-4843-88BF-E804A443100B}" name="48/1/2" totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="16">
+    <tableColumn id="1" xr3:uid="{80FFCD29-7FFB-4843-88BF-E804A443100B}" name="48/1/2" totalsRowFunction="custom" dataDxfId="37" totalsRowDxfId="36">
       <totalsRowFormula>AVERAGE(Table1214151942[48/1/2])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{CB857AE9-7A40-B24A-8805-7506FAE90C8B}" name="96/2/4" totalsRowFunction="average" dataDxfId="25" totalsRowDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{4359834E-C961-8F47-8E92-F4BCCDE23C4D}" name="192/4/8" totalsRowFunction="average" dataDxfId="24" totalsRowDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{7CF08588-9CC6-1F48-A9DD-1E58099385A1}" name="384/8/16" totalsRowFunction="average" dataDxfId="23" totalsRowDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{CB857AE9-7A40-B24A-8805-7506FAE90C8B}" name="96/2/4" totalsRowFunction="average" dataDxfId="35" totalsRowDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{4359834E-C961-8F47-8E92-F4BCCDE23C4D}" name="192/4/8" totalsRowFunction="average" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{7CF08588-9CC6-1F48-A9DD-1E58099385A1}" name="384/8/16" totalsRowFunction="average" dataDxfId="31" totalsRowDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{680FD551-31C1-3B4A-A986-A3047FFF7F09}" name="Table121415162053" displayName="Table121415162053" ref="J139:M150" totalsRowCount="1" headerRowDxfId="22" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{680FD551-31C1-3B4A-A986-A3047FFF7F09}" name="Table121415162053" displayName="Table121415162053" ref="J139:M150" totalsRowCount="1" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="J139:M149" xr:uid="{9A0998A7-66D7-E147-AE87-15B6065D5680}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -9298,19 +10982,59 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{DC37C131-5F5D-0D4E-BD10-6CC8ACC3AA71}" name="48/1/2" totalsRowFunction="custom" dataDxfId="21" totalsRowDxfId="11">
+    <tableColumn id="1" xr3:uid="{DC37C131-5F5D-0D4E-BD10-6CC8ACC3AA71}" name="48/1/2" totalsRowFunction="custom" dataDxfId="27" totalsRowDxfId="26">
       <totalsRowFormula>AVERAGE(Table121415162053[48/1/2])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{0D5AD745-3B14-2246-8E4D-3737E94C3424}" name="96/2/4" totalsRowFunction="average" dataDxfId="20" totalsRowDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{5E528244-6336-8C4A-B9DD-00D93BBBC769}" name="192/4/8" totalsRowFunction="average" dataDxfId="19" totalsRowDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{3F6E5AFC-81CA-4545-9EF3-6621EC1CBE68}" name="384/8/16" totalsRowFunction="average" dataDxfId="18" totalsRowDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{0D5AD745-3B14-2246-8E4D-3737E94C3424}" name="96/2/4" totalsRowFunction="average" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{5E528244-6336-8C4A-B9DD-00D93BBBC769}" name="192/4/8" totalsRowFunction="average" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{3F6E5AFC-81CA-4545-9EF3-6621EC1CBE68}" name="384/8/16" totalsRowFunction="average" dataDxfId="21" totalsRowDxfId="20"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{479F7965-3998-5D49-B11F-3DF0D24AAD15}" name="Table1214151946" displayName="Table1214151946" ref="C165:F176" totalsRowCount="1" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="C165:F175" xr:uid="{252395B1-FCBA-604D-947D-EC3CED3250D2}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{560C5431-9E7C-594F-94D1-38A5BB2A40BA}" name="48/1/2" totalsRowFunction="custom" dataDxfId="15" totalsRowDxfId="14">
+      <totalsRowFormula>AVERAGE(Table1214151946[48/1/2])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{D7D78837-32B5-4B47-B2EB-2A7953479D93}" name="96/2/4" totalsRowFunction="average" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{CEDC4E69-4D96-2E47-954C-56E3508B8983}" name="192/4/8" totalsRowFunction="average" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{5CBBD9D5-2AE5-D94A-B67E-B26FF3012E37}" name="384/8/16" totalsRowFunction="average" dataDxfId="9" totalsRowDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{43DCEAEF-EBDA-2B4E-8505-3C9554636F7A}" name="Table121415162057" displayName="Table121415162057" ref="J165:M176" totalsRowCount="1" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="J165:M175" xr:uid="{7657ECBD-E043-5542-90A4-BECD3CC767AF}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{58C2753F-F5E6-8B42-A667-28423163DFE6}" name="48/1/2" totalsRowFunction="custom" dataDxfId="7" totalsRowDxfId="3">
+      <totalsRowFormula>AVERAGE(Table121415162057[48/1/2])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{70DEBB54-4814-404A-A690-729BEE15B64B}" name="96/2/4" totalsRowFunction="average" dataDxfId="6" totalsRowDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{0D2A8966-2EBA-6347-AEFE-F81D2A1E797B}" name="192/4/8" totalsRowFunction="average" dataDxfId="5" totalsRowDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{C7B840E3-DF2D-6B4D-82D8-C265A8CFA334}" name="384/8/16" totalsRowFunction="average" dataDxfId="4" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{43882465-33C1-8E45-8C5B-6E2796C69C30}" name="Table1214" displayName="Table1214" ref="C8:F19" totalsRowCount="1" headerRowDxfId="117" dataDxfId="116">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{43882465-33C1-8E45-8C5B-6E2796C69C30}" name="Table1214" displayName="Table1214" ref="C8:F19" totalsRowCount="1" headerRowDxfId="137" dataDxfId="136">
   <autoFilter ref="C8:F18" xr:uid="{26D4EAA6-0F6B-D847-AC4C-A1E1EF972243}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -9318,19 +11042,19 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{ECEFB9F6-16FE-E04E-844A-AACC7B293BB2}" name="1/1/1" totalsRowFunction="custom" dataDxfId="115" totalsRowDxfId="114">
+    <tableColumn id="1" xr3:uid="{ECEFB9F6-16FE-E04E-844A-AACC7B293BB2}" name="1/1/1" totalsRowFunction="custom" dataDxfId="135" totalsRowDxfId="134">
       <totalsRowFormula>AVERAGE(Table1214[1/1/1])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{55F72C56-FCA4-AC43-B626-4AF6B7483939}" name="2/2/1" totalsRowFunction="average" dataDxfId="113" totalsRowDxfId="112"/>
-    <tableColumn id="3" xr3:uid="{7C069732-E830-8045-A0B0-B3BF291610EF}" name="4/4/1" totalsRowFunction="average" dataDxfId="111" totalsRowDxfId="110"/>
-    <tableColumn id="4" xr3:uid="{8CDDC8E9-E772-C14C-B2C1-6A75594F5FBE}" name="8/8/1" totalsRowFunction="average" dataDxfId="109" totalsRowDxfId="108"/>
+    <tableColumn id="2" xr3:uid="{55F72C56-FCA4-AC43-B626-4AF6B7483939}" name="2/2/1" totalsRowFunction="average" dataDxfId="133" totalsRowDxfId="132"/>
+    <tableColumn id="3" xr3:uid="{7C069732-E830-8045-A0B0-B3BF291610EF}" name="4/4/1" totalsRowFunction="average" dataDxfId="131" totalsRowDxfId="130"/>
+    <tableColumn id="4" xr3:uid="{8CDDC8E9-E772-C14C-B2C1-6A75594F5FBE}" name="8/8/1" totalsRowFunction="average" dataDxfId="129" totalsRowDxfId="128"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{FE766060-A7BD-2048-ABFD-3FD69B515A68}" name="Table121415" displayName="Table121415" ref="C35:H46" totalsRowCount="1" headerRowDxfId="107" dataDxfId="106">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{FE766060-A7BD-2048-ABFD-3FD69B515A68}" name="Table121415" displayName="Table121415" ref="C35:H46" totalsRowCount="1" headerRowDxfId="127" dataDxfId="126">
   <autoFilter ref="C35:H45" xr:uid="{B8E8E606-9A74-0D4F-AA01-6A7104D5FDDD}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -9340,21 +11064,21 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{5B90E881-6C60-454E-86BB-086695E6CAF8}" name="1/1/1" totalsRowFunction="custom" dataDxfId="105" totalsRowDxfId="104">
+    <tableColumn id="1" xr3:uid="{5B90E881-6C60-454E-86BB-086695E6CAF8}" name="1/1/1" totalsRowFunction="custom" dataDxfId="125" totalsRowDxfId="124">
       <totalsRowFormula>AVERAGE(Table121415[1/1/1])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{D531CACF-18B4-1041-B0C1-6D0252E32A8A}" name="2/2/1" totalsRowFunction="average" dataDxfId="103" totalsRowDxfId="102"/>
-    <tableColumn id="3" xr3:uid="{D0898416-43B5-3E4A-BDC1-7C89C1F0D5E0}" name="4/4/1" totalsRowFunction="average" dataDxfId="101" totalsRowDxfId="100"/>
-    <tableColumn id="4" xr3:uid="{4392AEA4-B357-F647-A208-E130D063C6E1}" name="8/8/1" totalsRowFunction="average" dataDxfId="99" totalsRowDxfId="98"/>
-    <tableColumn id="6" xr3:uid="{0A1338EF-4B77-1D48-8777-D4CA34460AB0}" name="16/16/1" totalsRowFunction="average" dataDxfId="97" totalsRowDxfId="96"/>
-    <tableColumn id="7" xr3:uid="{B90FEE84-6896-1641-8E20-B1872987B7BE}" name="32/32/2" totalsRowFunction="average" dataDxfId="95" totalsRowDxfId="94"/>
+    <tableColumn id="2" xr3:uid="{D531CACF-18B4-1041-B0C1-6D0252E32A8A}" name="2/2/1" totalsRowFunction="average" dataDxfId="123" totalsRowDxfId="122"/>
+    <tableColumn id="3" xr3:uid="{D0898416-43B5-3E4A-BDC1-7C89C1F0D5E0}" name="4/4/1" totalsRowFunction="average" dataDxfId="121" totalsRowDxfId="120"/>
+    <tableColumn id="4" xr3:uid="{4392AEA4-B357-F647-A208-E130D063C6E1}" name="8/8/1" totalsRowFunction="average" dataDxfId="119" totalsRowDxfId="118"/>
+    <tableColumn id="6" xr3:uid="{0A1338EF-4B77-1D48-8777-D4CA34460AB0}" name="16/16/1" totalsRowFunction="average" dataDxfId="117" totalsRowDxfId="116"/>
+    <tableColumn id="7" xr3:uid="{B90FEE84-6896-1641-8E20-B1872987B7BE}" name="32/32/2" totalsRowFunction="average" dataDxfId="115" totalsRowDxfId="114"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{C0771168-9D09-C749-AC55-A312881E4A86}" name="Table12141516" displayName="Table12141516" ref="L35:Q46" totalsRowCount="1" headerRowDxfId="93" dataDxfId="92">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{C0771168-9D09-C749-AC55-A312881E4A86}" name="Table12141516" displayName="Table12141516" ref="L35:Q46" totalsRowCount="1" headerRowDxfId="113" dataDxfId="112">
   <autoFilter ref="L35:Q45" xr:uid="{4EFDE026-18DB-0845-B41D-7D7B774A1B01}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -9364,21 +11088,21 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{3F8BB35C-BA7F-414F-98E1-50F3192CFD83}" name="1/1/1" totalsRowFunction="custom" dataDxfId="91" totalsRowDxfId="90">
+    <tableColumn id="1" xr3:uid="{3F8BB35C-BA7F-414F-98E1-50F3192CFD83}" name="1/1/1" totalsRowFunction="custom" dataDxfId="111" totalsRowDxfId="110">
       <totalsRowFormula>AVERAGE(Table12141516[1/1/1])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{070B7708-5F3C-5747-BB02-C79FC61D286A}" name="2/2/1" totalsRowFunction="average" dataDxfId="89" totalsRowDxfId="88"/>
-    <tableColumn id="3" xr3:uid="{58E0425E-3A2E-5C45-8330-41CFB638FBEE}" name="4/4/1" totalsRowFunction="average" dataDxfId="87" totalsRowDxfId="86"/>
-    <tableColumn id="4" xr3:uid="{21D6854D-0C08-4B4A-86CE-586C1F6F99EF}" name="8/8/1" totalsRowFunction="average" dataDxfId="85" totalsRowDxfId="84"/>
-    <tableColumn id="6" xr3:uid="{6E478822-1027-2D40-94B7-591A68C43394}" name="16/16/1" totalsRowFunction="average" dataDxfId="83" totalsRowDxfId="82"/>
-    <tableColumn id="7" xr3:uid="{063A683F-E92B-DC4C-8BF0-A3E1B5948664}" name="32/32/2" totalsRowFunction="average" dataDxfId="81" totalsRowDxfId="80"/>
+    <tableColumn id="2" xr3:uid="{070B7708-5F3C-5747-BB02-C79FC61D286A}" name="2/2/1" totalsRowFunction="average" dataDxfId="109" totalsRowDxfId="108"/>
+    <tableColumn id="3" xr3:uid="{58E0425E-3A2E-5C45-8330-41CFB638FBEE}" name="4/4/1" totalsRowFunction="average" dataDxfId="107" totalsRowDxfId="106"/>
+    <tableColumn id="4" xr3:uid="{21D6854D-0C08-4B4A-86CE-586C1F6F99EF}" name="8/8/1" totalsRowFunction="average" dataDxfId="105" totalsRowDxfId="104"/>
+    <tableColumn id="6" xr3:uid="{6E478822-1027-2D40-94B7-591A68C43394}" name="16/16/1" totalsRowFunction="average" dataDxfId="103" totalsRowDxfId="102"/>
+    <tableColumn id="7" xr3:uid="{063A683F-E92B-DC4C-8BF0-A3E1B5948664}" name="32/32/2" totalsRowFunction="average" dataDxfId="101" totalsRowDxfId="100"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{3A5DB260-BC51-9943-9AA6-EF26448D4AB0}" name="Table121417" displayName="Table121417" ref="C61:F72" totalsRowCount="1" headerRowDxfId="79" dataDxfId="78">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{3A5DB260-BC51-9943-9AA6-EF26448D4AB0}" name="Table121417" displayName="Table121417" ref="C61:F72" totalsRowCount="1" headerRowDxfId="99" dataDxfId="98">
   <autoFilter ref="C61:F71" xr:uid="{77973C46-8BAA-9E42-9CF9-1BC781EFFEBC}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -9386,19 +11110,19 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{611F1749-0588-F848-9620-3D32DE58D012}" name="1" totalsRowFunction="custom" dataDxfId="77" totalsRowDxfId="76">
+    <tableColumn id="1" xr3:uid="{611F1749-0588-F848-9620-3D32DE58D012}" name="1" totalsRowFunction="custom" dataDxfId="97" totalsRowDxfId="96">
       <totalsRowFormula>AVERAGE(Table121417[1])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5C8112FE-A4B8-2842-B70E-44A2DC4E2C86}" name="2" totalsRowFunction="average" dataDxfId="75" totalsRowDxfId="74"/>
-    <tableColumn id="3" xr3:uid="{4BB710EE-2F6B-104C-91C2-4D5DE8B5EA8D}" name="4" totalsRowFunction="average" dataDxfId="73" totalsRowDxfId="72"/>
-    <tableColumn id="4" xr3:uid="{A0144014-194E-4444-8B54-6D61F558C222}" name="8" totalsRowFunction="average" dataDxfId="71" totalsRowDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{5C8112FE-A4B8-2842-B70E-44A2DC4E2C86}" name="2" totalsRowFunction="average" dataDxfId="95" totalsRowDxfId="94"/>
+    <tableColumn id="3" xr3:uid="{4BB710EE-2F6B-104C-91C2-4D5DE8B5EA8D}" name="4" totalsRowFunction="average" dataDxfId="93" totalsRowDxfId="92"/>
+    <tableColumn id="4" xr3:uid="{A0144014-194E-4444-8B54-6D61F558C222}" name="8" totalsRowFunction="average" dataDxfId="91" totalsRowDxfId="90"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{31496C44-A2F7-6046-A581-DE00E1A64495}" name="Table12141718" displayName="Table12141718" ref="L61:O72" totalsRowCount="1" headerRowDxfId="69" dataDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{31496C44-A2F7-6046-A581-DE00E1A64495}" name="Table12141718" displayName="Table12141718" ref="L61:O72" totalsRowCount="1" headerRowDxfId="89" dataDxfId="88">
   <autoFilter ref="L61:O71" xr:uid="{2A271704-5B21-F64E-8049-792EF620B77A}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -9406,19 +11130,19 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D743CB9F-8265-124F-92C6-6757D444A101}" name="1" totalsRowFunction="custom" dataDxfId="67" totalsRowDxfId="66">
+    <tableColumn id="1" xr3:uid="{D743CB9F-8265-124F-92C6-6757D444A101}" name="1" totalsRowFunction="custom" dataDxfId="87" totalsRowDxfId="86">
       <totalsRowFormula>AVERAGE(Table12141718[1])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5C8613A6-D77C-1E41-8FFD-A8DB9B432EFA}" name="2" totalsRowFunction="average" dataDxfId="65" totalsRowDxfId="64"/>
-    <tableColumn id="3" xr3:uid="{844C3824-E977-A14C-8C1A-147CFABDF145}" name="4" totalsRowFunction="average" dataDxfId="63" totalsRowDxfId="62"/>
-    <tableColumn id="4" xr3:uid="{245E9196-FB1E-2B4A-926B-2633671BC3A4}" name="8" totalsRowFunction="average" dataDxfId="61" totalsRowDxfId="60"/>
+    <tableColumn id="2" xr3:uid="{5C8613A6-D77C-1E41-8FFD-A8DB9B432EFA}" name="2" totalsRowFunction="average" dataDxfId="85" totalsRowDxfId="84"/>
+    <tableColumn id="3" xr3:uid="{844C3824-E977-A14C-8C1A-147CFABDF145}" name="4" totalsRowFunction="average" dataDxfId="83" totalsRowDxfId="82"/>
+    <tableColumn id="4" xr3:uid="{245E9196-FB1E-2B4A-926B-2633671BC3A4}" name="8" totalsRowFunction="average" dataDxfId="81" totalsRowDxfId="80"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{D5DB36BD-3777-BD47-B388-C694D27FBE74}" name="Table12141519" displayName="Table12141519" ref="C87:F98" totalsRowCount="1" headerRowDxfId="59" dataDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{D5DB36BD-3777-BD47-B388-C694D27FBE74}" name="Table12141519" displayName="Table12141519" ref="C87:F98" totalsRowCount="1" headerRowDxfId="79" dataDxfId="78">
   <autoFilter ref="C87:F97" xr:uid="{1F757434-E3E5-594B-8FFA-2545970AF61F}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -9426,19 +11150,19 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9E17C061-277B-7145-AC08-E3828B5A8FB5}" name="56/1/2" totalsRowFunction="custom" dataDxfId="57" totalsRowDxfId="3">
+    <tableColumn id="1" xr3:uid="{9E17C061-277B-7145-AC08-E3828B5A8FB5}" name="56/1/2" totalsRowFunction="custom" dataDxfId="77" totalsRowDxfId="76">
       <totalsRowFormula>AVERAGE(Table12141519[56/1/2])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{49DD9B33-6A59-EC46-9C7E-E574A972BCE4}" name="112/2/4" totalsRowFunction="average" dataDxfId="56" totalsRowDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{7C11F312-D5FE-DE47-9FE3-98A59213BB44}" name="224/4/8" totalsRowFunction="average" dataDxfId="55" totalsRowDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{505390BD-3EED-7C4E-811B-893A241116FD}" name="448/8/16" totalsRowFunction="average" dataDxfId="54" totalsRowDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{49DD9B33-6A59-EC46-9C7E-E574A972BCE4}" name="112/2/4" totalsRowFunction="average" dataDxfId="75" totalsRowDxfId="74"/>
+    <tableColumn id="3" xr3:uid="{7C11F312-D5FE-DE47-9FE3-98A59213BB44}" name="224/4/8" totalsRowFunction="average" dataDxfId="73" totalsRowDxfId="72"/>
+    <tableColumn id="4" xr3:uid="{505390BD-3EED-7C4E-811B-893A241116FD}" name="448/8/16" totalsRowFunction="average" dataDxfId="71" totalsRowDxfId="70"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{6588BB5D-67F0-BB43-9F21-59AFA57E8AF4}" name="Table1214151620" displayName="Table1214151620" ref="J87:M98" totalsRowCount="1" headerRowDxfId="53" dataDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{6588BB5D-67F0-BB43-9F21-59AFA57E8AF4}" name="Table1214151620" displayName="Table1214151620" ref="J87:M98" totalsRowCount="1" headerRowDxfId="69" dataDxfId="68">
   <autoFilter ref="J87:M97" xr:uid="{5512B521-6B77-F843-A5B4-F0AB0FB6DFB5}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -9446,19 +11170,19 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{DB504DAF-52D8-1649-87BC-A7AB49A17859}" name="56/1/2" totalsRowFunction="custom" dataDxfId="51" totalsRowDxfId="7">
+    <tableColumn id="1" xr3:uid="{DB504DAF-52D8-1649-87BC-A7AB49A17859}" name="56/1/2" totalsRowFunction="custom" dataDxfId="67" totalsRowDxfId="66">
       <totalsRowFormula>AVERAGE(Table1214151620[56/1/2])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{EC6E11B1-7660-A14C-98A7-F5546CF00337}" name="112/2/4" totalsRowFunction="average" dataDxfId="50" totalsRowDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{209F27B7-05A6-E84B-99C5-22633169F39F}" name="224/4/8" totalsRowFunction="average" dataDxfId="49" totalsRowDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{8A07B38D-10AE-B547-8DB0-B10F4A88768B}" name="448/8/16" totalsRowFunction="average" dataDxfId="48" totalsRowDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{EC6E11B1-7660-A14C-98A7-F5546CF00337}" name="112/2/4" totalsRowFunction="average" dataDxfId="65" totalsRowDxfId="64"/>
+    <tableColumn id="3" xr3:uid="{209F27B7-05A6-E84B-99C5-22633169F39F}" name="224/4/8" totalsRowFunction="average" dataDxfId="63" totalsRowDxfId="62"/>
+    <tableColumn id="4" xr3:uid="{8A07B38D-10AE-B547-8DB0-B10F4A88768B}" name="448/8/16" totalsRowFunction="average" dataDxfId="61" totalsRowDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{443C52A3-984F-2F45-AC25-3FF834E387F5}" name="Table121415194" displayName="Table121415194" ref="C113:F124" totalsRowCount="1" headerRowDxfId="47" dataDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{443C52A3-984F-2F45-AC25-3FF834E387F5}" name="Table121415194" displayName="Table121415194" ref="C113:F124" totalsRowCount="1" headerRowDxfId="59" dataDxfId="58">
   <autoFilter ref="C113:F123" xr:uid="{BADBF933-19E9-6F49-B79D-95C8A79A3C27}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -9466,12 +11190,12 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{98F9AAF6-7D4C-C94D-92F3-F62953919301}" name="48/1/2" totalsRowFunction="custom" dataDxfId="45" totalsRowDxfId="44">
+    <tableColumn id="1" xr3:uid="{98F9AAF6-7D4C-C94D-92F3-F62953919301}" name="48/1/2" totalsRowFunction="custom" dataDxfId="57" totalsRowDxfId="56">
       <totalsRowFormula>AVERAGE(Table121415194[48/1/2])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{EE88288C-1811-744F-A47E-F666E41AFEBA}" name="96/2/4" totalsRowFunction="average" dataDxfId="43" totalsRowDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{D30EAA85-D358-D547-ABB8-61D1166DE7CE}" name="192/4/8" totalsRowFunction="average" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{7CF5ACA5-A5FD-1C42-8AFE-7C2BD7973668}" name="384/8/16" totalsRowFunction="average" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{EE88288C-1811-744F-A47E-F666E41AFEBA}" name="96/2/4" totalsRowFunction="average" dataDxfId="55" totalsRowDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{D30EAA85-D358-D547-ABB8-61D1166DE7CE}" name="192/4/8" totalsRowFunction="average" dataDxfId="53" totalsRowDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{7CF5ACA5-A5FD-1C42-8AFE-7C2BD7973668}" name="384/8/16" totalsRowFunction="average" dataDxfId="51" totalsRowDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -9774,10 +11498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CACD4666-87E2-F84B-9806-2702F4658363}">
-  <dimension ref="A1:AG151"/>
+  <dimension ref="A1:AG177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="P89" sqref="P89"/>
+    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
+      <selection activeCell="P180" sqref="P180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12246,7 +13970,7 @@
         <v>137.07</v>
       </c>
     </row>
-    <row r="145" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B145" s="10"/>
       <c r="C145">
         <v>4.01</v>
@@ -12274,7 +13998,7 @@
         <v>150.61000000000001</v>
       </c>
     </row>
-    <row r="146" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B146" s="10"/>
       <c r="C146">
         <v>3.69</v>
@@ -12302,7 +14026,7 @@
         <v>140.96</v>
       </c>
     </row>
-    <row r="147" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B147" s="10"/>
       <c r="C147">
         <v>3.23</v>
@@ -12330,7 +14054,7 @@
         <v>152.49</v>
       </c>
     </row>
-    <row r="148" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B148" s="10"/>
       <c r="C148">
         <v>3.79</v>
@@ -12358,7 +14082,7 @@
         <v>143.66</v>
       </c>
     </row>
-    <row r="149" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B149" s="10"/>
       <c r="C149">
         <v>3.4</v>
@@ -12386,7 +14110,7 @@
         <v>152.9</v>
       </c>
     </row>
-    <row r="150" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B150" s="5" t="s">
         <v>9</v>
       </c>
@@ -12426,7 +14150,7 @@
         <v>145.25900000000004</v>
       </c>
     </row>
-    <row r="151" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B151" s="5" t="s">
         <v>10</v>
       </c>
@@ -12468,8 +14192,410 @@
         <v>5.2349900774606217</v>
       </c>
     </row>
+    <row r="158" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A158" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B158" s="3"/>
+      <c r="C158" s="2"/>
+      <c r="D158" s="2"/>
+    </row>
+    <row r="165" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="C165" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D165" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E165" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F165" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J165" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K165" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L165" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M165" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="166" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B166" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C166">
+        <v>4.8</v>
+      </c>
+      <c r="D166">
+        <v>9.5500000000000007</v>
+      </c>
+      <c r="E166">
+        <v>50.17</v>
+      </c>
+      <c r="F166">
+        <v>93.39</v>
+      </c>
+      <c r="I166" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J166">
+        <v>4.26</v>
+      </c>
+      <c r="K166">
+        <v>9.99</v>
+      </c>
+      <c r="L166">
+        <v>34.31</v>
+      </c>
+      <c r="M166">
+        <v>89.56</v>
+      </c>
+    </row>
+    <row r="167" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B167" s="10"/>
+      <c r="C167">
+        <v>5.81</v>
+      </c>
+      <c r="D167">
+        <v>10.16</v>
+      </c>
+      <c r="E167">
+        <v>27.43</v>
+      </c>
+      <c r="F167">
+        <v>88.43</v>
+      </c>
+      <c r="I167" s="10"/>
+      <c r="J167">
+        <v>5.65</v>
+      </c>
+      <c r="K167">
+        <v>13.01</v>
+      </c>
+      <c r="L167">
+        <v>33.78</v>
+      </c>
+      <c r="M167">
+        <v>93.68</v>
+      </c>
+    </row>
+    <row r="168" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B168" s="10"/>
+      <c r="C168">
+        <v>3.61</v>
+      </c>
+      <c r="D168">
+        <v>9.34</v>
+      </c>
+      <c r="E168">
+        <v>27.71</v>
+      </c>
+      <c r="F168">
+        <v>87.41</v>
+      </c>
+      <c r="I168" s="10"/>
+      <c r="J168">
+        <v>4.34</v>
+      </c>
+      <c r="K168">
+        <v>10.1</v>
+      </c>
+      <c r="L168">
+        <v>46.18</v>
+      </c>
+      <c r="M168">
+        <v>101.8</v>
+      </c>
+    </row>
+    <row r="169" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B169" s="10"/>
+      <c r="C169">
+        <v>3.84</v>
+      </c>
+      <c r="D169">
+        <v>9.6</v>
+      </c>
+      <c r="E169">
+        <v>26.55</v>
+      </c>
+      <c r="F169">
+        <v>91.08</v>
+      </c>
+      <c r="I169" s="10"/>
+      <c r="J169">
+        <v>3.92</v>
+      </c>
+      <c r="K169">
+        <v>10.11</v>
+      </c>
+      <c r="L169">
+        <v>28.35</v>
+      </c>
+      <c r="M169">
+        <v>83.35</v>
+      </c>
+    </row>
+    <row r="170" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B170" s="10"/>
+      <c r="C170">
+        <v>4.92</v>
+      </c>
+      <c r="D170">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="E170">
+        <v>28.57</v>
+      </c>
+      <c r="F170">
+        <v>114.01</v>
+      </c>
+      <c r="I170" s="10"/>
+      <c r="J170">
+        <v>3.86</v>
+      </c>
+      <c r="K170">
+        <v>10.39</v>
+      </c>
+      <c r="L170">
+        <v>29.76</v>
+      </c>
+      <c r="M170">
+        <v>89.19</v>
+      </c>
+    </row>
+    <row r="171" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B171" s="10"/>
+      <c r="C171">
+        <v>4.13</v>
+      </c>
+      <c r="D171">
+        <v>9.61</v>
+      </c>
+      <c r="E171">
+        <v>46.28</v>
+      </c>
+      <c r="F171">
+        <v>94.72</v>
+      </c>
+      <c r="I171" s="10"/>
+      <c r="J171">
+        <v>4.26</v>
+      </c>
+      <c r="K171">
+        <v>10.58</v>
+      </c>
+      <c r="L171">
+        <v>30.37</v>
+      </c>
+      <c r="M171">
+        <v>94.73</v>
+      </c>
+    </row>
+    <row r="172" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B172" s="10"/>
+      <c r="C172">
+        <v>4.83</v>
+      </c>
+      <c r="D172">
+        <v>9.6</v>
+      </c>
+      <c r="E172">
+        <v>26.56</v>
+      </c>
+      <c r="F172">
+        <v>107.57</v>
+      </c>
+      <c r="I172" s="10"/>
+      <c r="J172">
+        <v>5.05</v>
+      </c>
+      <c r="K172">
+        <v>9.6</v>
+      </c>
+      <c r="L172">
+        <v>31.8</v>
+      </c>
+      <c r="M172">
+        <v>98.57</v>
+      </c>
+    </row>
+    <row r="173" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B173" s="10"/>
+      <c r="C173">
+        <v>5.37</v>
+      </c>
+      <c r="D173">
+        <v>9.6300000000000008</v>
+      </c>
+      <c r="E173">
+        <v>28.26</v>
+      </c>
+      <c r="F173">
+        <v>102.38</v>
+      </c>
+      <c r="I173" s="10"/>
+      <c r="J173">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="K173">
+        <v>11.77</v>
+      </c>
+      <c r="L173">
+        <v>32.99</v>
+      </c>
+      <c r="M173">
+        <v>110.94</v>
+      </c>
+    </row>
+    <row r="174" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B174" s="10"/>
+      <c r="C174">
+        <v>4.8099999999999996</v>
+      </c>
+      <c r="D174">
+        <v>9.34</v>
+      </c>
+      <c r="E174">
+        <v>37.28</v>
+      </c>
+      <c r="F174">
+        <v>105.38</v>
+      </c>
+      <c r="I174" s="10"/>
+      <c r="J174">
+        <v>10.44</v>
+      </c>
+      <c r="K174">
+        <v>9.89</v>
+      </c>
+      <c r="L174">
+        <v>32.75</v>
+      </c>
+      <c r="M174">
+        <v>110.9</v>
+      </c>
+    </row>
+    <row r="175" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B175" s="10"/>
+      <c r="C175">
+        <v>4.26</v>
+      </c>
+      <c r="D175">
+        <v>10.78</v>
+      </c>
+      <c r="E175">
+        <v>28.96</v>
+      </c>
+      <c r="F175">
+        <v>92.31</v>
+      </c>
+      <c r="I175" s="10"/>
+      <c r="J175">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="K175">
+        <v>10.050000000000001</v>
+      </c>
+      <c r="L175">
+        <v>33.99</v>
+      </c>
+      <c r="M175">
+        <v>122.27</v>
+      </c>
+    </row>
+    <row r="176" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B176" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C176" s="6">
+        <f>AVERAGE(Table1214151946[48/1/2])</f>
+        <v>4.6379999999999999</v>
+      </c>
+      <c r="D176" s="6">
+        <f>SUBTOTAL(101,Table1214151946[96/2/4])</f>
+        <v>9.7809999999999988</v>
+      </c>
+      <c r="E176" s="6">
+        <f>SUBTOTAL(101,Table1214151946[192/4/8])</f>
+        <v>32.777000000000001</v>
+      </c>
+      <c r="F176" s="6">
+        <f>SUBTOTAL(101,Table1214151946[384/8/16])</f>
+        <v>97.667999999999978</v>
+      </c>
+      <c r="I176" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J176" s="6">
+        <f>AVERAGE(Table121415162057[48/1/2])</f>
+        <v>5.1280000000000001</v>
+      </c>
+      <c r="K176" s="6">
+        <f>SUBTOTAL(101,Table121415162057[96/2/4])</f>
+        <v>10.548999999999999</v>
+      </c>
+      <c r="L176" s="6">
+        <f>SUBTOTAL(101,Table121415162057[192/4/8])</f>
+        <v>33.428000000000004</v>
+      </c>
+      <c r="M176" s="6">
+        <f>SUBTOTAL(101,Table121415162057[384/8/16])</f>
+        <v>99.498999999999995</v>
+      </c>
+    </row>
+    <row r="177" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B177" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C177" s="7">
+        <f>STDEV(C166:C175)</f>
+        <v>0.6811885038502794</v>
+      </c>
+      <c r="D177" s="7">
+        <f t="shared" ref="D177:F177" si="10">STDEV(D166:D175)</f>
+        <v>0.45668978043695629</v>
+      </c>
+      <c r="E177" s="7">
+        <f t="shared" si="10"/>
+        <v>8.752698694942266</v>
+      </c>
+      <c r="F177" s="7">
+        <f t="shared" si="10"/>
+        <v>9.0459171883108542</v>
+      </c>
+      <c r="G177" s="7"/>
+      <c r="H177" s="7"/>
+      <c r="I177" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J177" s="7">
+        <f>STDEV(J166:J175)</f>
+        <v>1.9435523032724265</v>
+      </c>
+      <c r="K177" s="7">
+        <f t="shared" ref="K177:M177" si="11">STDEV(K166:K175)</f>
+        <v>1.0469155754989139</v>
+      </c>
+      <c r="L177" s="7">
+        <f t="shared" si="11"/>
+        <v>4.895857205615548</v>
+      </c>
+      <c r="M177" s="7">
+        <f t="shared" si="11"/>
+        <v>12.055468514790807</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="14">
+    <mergeCell ref="B166:B175"/>
+    <mergeCell ref="I166:I175"/>
     <mergeCell ref="B140:B149"/>
     <mergeCell ref="I140:I149"/>
     <mergeCell ref="K9:K18"/>
@@ -12485,7 +14611,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <tableParts count="12">
+  <tableParts count="14">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -12498,6 +14624,8 @@
     <tablePart r:id="rId11"/>
     <tablePart r:id="rId12"/>
     <tablePart r:id="rId13"/>
+    <tablePart r:id="rId14"/>
+    <tablePart r:id="rId15"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>